<commit_message>
uh update to array analysis
</commit_message>
<xml_diff>
--- a/Project 2/JavaImpl/Lab2/Analysis2.xlsx
+++ b/Project 2/JavaImpl/Lab2/Analysis2.xlsx
@@ -2,26 +2,27 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiann\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\NTUwork\SC2001\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3090B371-88C1-4E4D-8A01-42DB1326A40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC507B0-6E19-4A95-B075-C4B0E76D2905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1E6B9D57-98B4-4DC0-9C08-6B8F636F6188}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{1E6B9D57-98B4-4DC0-9C08-6B8F636F6188}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualization" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$I$1:$M$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="409" r:id="rId3"/>
+    <pivotCache cacheId="170" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="51">
   <si>
     <t>Array</t>
   </si>
@@ -127,90 +128,6 @@
     <t> min-priority queue has complexity Θ(V + E log V).</t>
   </si>
   <si>
-    <t>Dense,10,Array,146,13446300</t>
-  </si>
-  <si>
-    <t>Dense,10,Heap,213,1594800</t>
-  </si>
-  <si>
-    <t>Dense,100,Array,20542,3327500</t>
-  </si>
-  <si>
-    <t>Dense,100,Heap,12143,2649700</t>
-  </si>
-  <si>
-    <t>Dense,1000,Array,2267712,37633000</t>
-  </si>
-  <si>
-    <t>Dense,1000,Heap,1027040,54418000</t>
-  </si>
-  <si>
-    <t>Dense,20,Array,789,370700</t>
-  </si>
-  <si>
-    <t>Dense,20,Heap,740,513900</t>
-  </si>
-  <si>
-    <t>Dense,40,Array,3217,277600</t>
-  </si>
-  <si>
-    <t>Dense,40,Heap,2266,480300</t>
-  </si>
-  <si>
-    <t>Dense,500,Array,566978,3695400</t>
-  </si>
-  <si>
-    <t>Dense,500,Heap,262592,6060300</t>
-  </si>
-  <si>
-    <t>Dense,5000,Array,56953404,214762700</t>
-  </si>
-  <si>
-    <t>Dense,5000,Heap,25158844,456790100</t>
-  </si>
-  <si>
-    <t>Sparse,10,Array,136,222900</t>
-  </si>
-  <si>
-    <t>Sparse,10,Heap,132,229200</t>
-  </si>
-  <si>
-    <t>Sparse,100,Array,19996,955900</t>
-  </si>
-  <si>
-    <t>Sparse,100,Heap,6893,790100</t>
-  </si>
-  <si>
-    <t>Sparse,1000,Array,2282587,14185300</t>
-  </si>
-  <si>
-    <t>Sparse,1000,Heap,485108,22441400</t>
-  </si>
-  <si>
-    <t>Sparse,20,Array,590,131000</t>
-  </si>
-  <si>
-    <t>Sparse,20,Heap,491,168900</t>
-  </si>
-  <si>
-    <t>Sparse,40,Array,2718,216800</t>
-  </si>
-  <si>
-    <t>Sparse,40,Heap,1439,348100</t>
-  </si>
-  <si>
-    <t>Sparse,500,Array,541504,3157700</t>
-  </si>
-  <si>
-    <t>Sparse,500,Heap,126910,2679600</t>
-  </si>
-  <si>
-    <t>Sparse,5000,Array,59840404,267353500</t>
-  </si>
-  <si>
-    <t>Sparse,5000,Heap,11407621,177443600</t>
-  </si>
-  <si>
     <t>Array-theoretically</t>
   </si>
   <si>
@@ -219,12 +136,96 @@
   <si>
     <t/>
   </si>
+  <si>
+    <t>Dense,10,Array,222,12311800</t>
+  </si>
+  <si>
+    <t>Dense,10,Heap,213,1774100</t>
+  </si>
+  <si>
+    <t>Dense,100,Array,35277,2886900</t>
+  </si>
+  <si>
+    <t>Dense,100,Heap,12143,2933400</t>
+  </si>
+  <si>
+    <t>Dense,1000,Array,4029793,32070100</t>
+  </si>
+  <si>
+    <t>Dense,1000,Heap,1027040,64510700</t>
+  </si>
+  <si>
+    <t>Dense,20,Array,1253,257200</t>
+  </si>
+  <si>
+    <t>Dense,20,Heap,740,333200</t>
+  </si>
+  <si>
+    <t>Dense,40,Array,5352,257800</t>
+  </si>
+  <si>
+    <t>Dense,40,Heap,2266,532000</t>
+  </si>
+  <si>
+    <t>Dense,500,Array,1016877,3049200</t>
+  </si>
+  <si>
+    <t>Dense,500,Heap,262592,7701500</t>
+  </si>
+  <si>
+    <t>Dense,5000,Array,100834480,88495300</t>
+  </si>
+  <si>
+    <t>Dense,5000,Heap,25158844,404758400</t>
+  </si>
+  <si>
+    <t>Sparse,10,Array,198,215400</t>
+  </si>
+  <si>
+    <t>Sparse,10,Heap,132,255400</t>
+  </si>
+  <si>
+    <t>Sparse,100,Array,35021,485200</t>
+  </si>
+  <si>
+    <t>Sparse,100,Heap,6893,772300</t>
+  </si>
+  <si>
+    <t>Sparse,1000,Array,4190113,6194100</t>
+  </si>
+  <si>
+    <t>Sparse,1000,Heap,485108,13952300</t>
+  </si>
+  <si>
+    <t>Sparse,20,Array,965,129900</t>
+  </si>
+  <si>
+    <t>Sparse,20,Heap,491,214900</t>
+  </si>
+  <si>
+    <t>Sparse,40,Array,4540,169200</t>
+  </si>
+  <si>
+    <t>Sparse,40,Heap,1439,177900</t>
+  </si>
+  <si>
+    <t>Sparse,500,Array,982006,1720200</t>
+  </si>
+  <si>
+    <t>Sparse,500,Heap,126910,2184900</t>
+  </si>
+  <si>
+    <t>Sparse,5000,Array,110211671,152229900</t>
+  </si>
+  <si>
+    <t>Sparse,5000,Heap,11407621,199905000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,16 +251,35 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -278,23 +298,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF252525"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF252525"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF252525"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF252525"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF252525"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1459,7 +1512,6 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1516,7 +1568,6 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1611,6 +1662,9 @@
       <c:pivotFmt>
         <c:idx val="22"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:srgbClr val="7030A0"/>
@@ -1668,6 +1722,9 @@
       <c:pivotFmt>
         <c:idx val="23"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1725,6 +1782,9 @@
       <c:pivotFmt>
         <c:idx val="24"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent4">
@@ -1828,7 +1888,6 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1886,7 +1945,6 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1966,25 +2024,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>146</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>789</c:v>
+                  <c:v>1253</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3217</c:v>
+                  <c:v>5352</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20542</c:v>
+                  <c:v>35277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>566978</c:v>
+                  <c:v>1016877</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2267712</c:v>
+                  <c:v>4029793</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56953404</c:v>
+                  <c:v>100834480</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2002,6 +2060,98 @@
           <c:tx>
             <c:strRef>
               <c:f>Visualization!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Visualization!$A$5:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Visualization!$C$5:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12143</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>262592</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1027040</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25158844</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B342-48A5-B309-1EC9CF3EEE70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Visualization!$D$3:$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2054,30 +2204,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Visualization!$C$5:$C$12</c:f>
+              <c:f>Visualization!$D$5:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>300</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1200</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4800</c:v>
+                  <c:v>6400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30000</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>750000</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3000000</c:v>
+                  <c:v>4000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75000000</c:v>
+                  <c:v>100000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2085,12 +2235,104 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B342-48A5-B309-1EC9CF3EEE70}"/>
+              <c16:uniqueId val="{00000000-B1DE-4C84-84A5-E0AA04749FFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Visualization!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heap-theoretically</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Visualization!$A$5:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Visualization!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>232.8771237954945</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>745.75424759098905</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2451.5084951819781</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12657.54247590989</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>267931.56856932415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1039863.1371386483</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25245754.247590989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B1DE-4C84-84A5-E0AA04749FFC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2390,6 +2632,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2446,6 +2691,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2502,6 +2750,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2615,6 +2866,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2642,6 +2896,9 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:srgbClr val="7030A0"/>
@@ -2699,6 +2956,9 @@
       <c:pivotFmt>
         <c:idx val="6"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent4">
@@ -2964,25 +3224,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>136</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>590</c:v>
+                  <c:v>965</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2718</c:v>
+                  <c:v>4540</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19996</c:v>
+                  <c:v>35021</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>541504</c:v>
+                  <c:v>982006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2282587</c:v>
+                  <c:v>4190113</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59840404</c:v>
+                  <c:v>110211671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3149,25 +3409,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>202</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>788</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3034</c:v>
+                  <c:v>6400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19088</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>474972</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1900388</c:v>
+                  <c:v>4000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47489502</c:v>
+                  <c:v>100000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3242,25 +3502,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>84.219280948873632</c:v>
+                  <c:v>164.44850683942991</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>280.43856189774726</c:v>
+                  <c:v>497.99651368748511</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>929.87712379549453</c:v>
+                  <c:v>1475.8663446961523</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5208.3856189774724</c:v>
+                  <c:v>6973.9494239009364</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>116968.89214233104</c:v>
+                  <c:v>129265.38592932424</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>460159.78428466211</c:v>
+                  <c:v>487754.37460742478</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11306189.561897747</c:v>
+                  <c:v>11478978.483791253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3622,7 +3882,6 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3691,7 +3950,6 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3706,6 +3964,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3775,6 +4036,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3842,6 +4106,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3986,25 +4253,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13446300</c:v>
+                  <c:v>12311800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>370700</c:v>
+                  <c:v>257200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>277600</c:v>
+                  <c:v>257800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3327500</c:v>
+                  <c:v>2886900</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3695400</c:v>
+                  <c:v>3049200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37633000</c:v>
+                  <c:v>32070100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>214762700</c:v>
+                  <c:v>88495300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4090,25 +4357,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1594800</c:v>
+                  <c:v>1774100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>513900</c:v>
+                  <c:v>333200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>480300</c:v>
+                  <c:v>532000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2649700</c:v>
+                  <c:v>2933400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6060300</c:v>
+                  <c:v>7701500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54418000</c:v>
+                  <c:v>64510700</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>456790100</c:v>
+                  <c:v>404758400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4121,7 +4388,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4465,9 +4731,8 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -4522,9 +4787,8 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -4537,6 +4801,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4594,6 +4861,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4609,6 +4879,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4666,6 +4939,9 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4752,64 +5028,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Visualization!$A$45:$A$52</c:f>
@@ -4846,25 +5064,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>222900</c:v>
+                  <c:v>215400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>131000</c:v>
+                  <c:v>129900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>216800</c:v>
+                  <c:v>169200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>955900</c:v>
+                  <c:v>485200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3157700</c:v>
+                  <c:v>1720200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14185300</c:v>
+                  <c:v>6194100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>267353500</c:v>
+                  <c:v>152229900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4902,64 +5120,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Visualization!$A$45:$A$52</c:f>
@@ -4996,25 +5156,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>229200</c:v>
+                  <c:v>255400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>168900</c:v>
+                  <c:v>214900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>348100</c:v>
+                  <c:v>177900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>790100</c:v>
+                  <c:v>772300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2679600</c:v>
+                  <c:v>2184900</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22441400</c:v>
+                  <c:v>13952300</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>177443600</c:v>
+                  <c:v>199905000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5027,9 +5187,8 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -7619,7 +7778,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kiann" refreshedDate="44837.986740856482" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="56" xr:uid="{C1740812-440E-4F27-B842-754C89F7B27F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kiann" refreshedDate="44838.706936574075" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="56" xr:uid="{C1740812-440E-4F27-B842-754C89F7B27F}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -7658,10 +7817,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Key Comparison" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="84.219280948873632" maxValue="75000000"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="132" maxValue="110211671"/>
     </cacheField>
     <cacheField name="Time (NS)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="131000" maxValue="456790100"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="129900" maxValue="404758400"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -7679,8 +7838,8 @@
     <x v="0"/>
     <n v="100"/>
     <x v="0"/>
-    <n v="146"/>
-    <n v="13446300"/>
+    <n v="222"/>
+    <n v="12311800"/>
   </r>
   <r>
     <x v="0"/>
@@ -7688,15 +7847,15 @@
     <n v="100"/>
     <x v="1"/>
     <n v="213"/>
-    <n v="1594800"/>
+    <n v="1774100"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="10000"/>
     <x v="0"/>
-    <n v="20542"/>
-    <n v="3327500"/>
+    <n v="35277"/>
+    <n v="2886900"/>
   </r>
   <r>
     <x v="0"/>
@@ -7704,15 +7863,15 @@
     <n v="10000"/>
     <x v="1"/>
     <n v="12143"/>
-    <n v="2649700"/>
+    <n v="2933400"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <n v="1000000"/>
     <x v="0"/>
-    <n v="2267712"/>
-    <n v="37633000"/>
+    <n v="4029793"/>
+    <n v="32070100"/>
   </r>
   <r>
     <x v="0"/>
@@ -7720,15 +7879,15 @@
     <n v="1000000"/>
     <x v="1"/>
     <n v="1027040"/>
-    <n v="54418000"/>
+    <n v="64510700"/>
   </r>
   <r>
     <x v="0"/>
     <x v="3"/>
     <n v="400"/>
     <x v="0"/>
-    <n v="789"/>
-    <n v="370700"/>
+    <n v="1253"/>
+    <n v="257200"/>
   </r>
   <r>
     <x v="0"/>
@@ -7736,15 +7895,15 @@
     <n v="400"/>
     <x v="1"/>
     <n v="740"/>
-    <n v="513900"/>
+    <n v="333200"/>
   </r>
   <r>
     <x v="0"/>
     <x v="4"/>
     <n v="1600"/>
     <x v="0"/>
-    <n v="3217"/>
-    <n v="277600"/>
+    <n v="5352"/>
+    <n v="257800"/>
   </r>
   <r>
     <x v="0"/>
@@ -7752,15 +7911,15 @@
     <n v="1600"/>
     <x v="1"/>
     <n v="2266"/>
-    <n v="480300"/>
+    <n v="532000"/>
   </r>
   <r>
     <x v="0"/>
     <x v="5"/>
     <n v="250000"/>
     <x v="0"/>
-    <n v="566978"/>
-    <n v="3695400"/>
+    <n v="1016877"/>
+    <n v="3049200"/>
   </r>
   <r>
     <x v="0"/>
@@ -7768,15 +7927,15 @@
     <n v="250000"/>
     <x v="1"/>
     <n v="262592"/>
-    <n v="6060300"/>
+    <n v="7701500"/>
   </r>
   <r>
     <x v="0"/>
     <x v="6"/>
     <n v="25000000"/>
     <x v="0"/>
-    <n v="56953404"/>
-    <n v="214762700"/>
+    <n v="100834480"/>
+    <n v="88495300"/>
   </r>
   <r>
     <x v="0"/>
@@ -7784,15 +7943,15 @@
     <n v="25000000"/>
     <x v="1"/>
     <n v="25158844"/>
-    <n v="456790100"/>
+    <n v="404758400"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <n v="51"/>
     <x v="0"/>
-    <n v="136"/>
-    <n v="222900"/>
+    <n v="198"/>
+    <n v="215400"/>
   </r>
   <r>
     <x v="1"/>
@@ -7800,15 +7959,15 @@
     <n v="51"/>
     <x v="1"/>
     <n v="132"/>
-    <n v="229200"/>
+    <n v="255400"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="4544"/>
     <x v="0"/>
-    <n v="19996"/>
-    <n v="955900"/>
+    <n v="35021"/>
+    <n v="485200"/>
   </r>
   <r>
     <x v="1"/>
@@ -7816,15 +7975,15 @@
     <n v="4544"/>
     <x v="1"/>
     <n v="6893"/>
-    <n v="790100"/>
+    <n v="772300"/>
   </r>
   <r>
     <x v="1"/>
     <x v="2"/>
     <n v="450194"/>
     <x v="0"/>
-    <n v="2282587"/>
-    <n v="14185300"/>
+    <n v="4190113"/>
+    <n v="6194100"/>
   </r>
   <r>
     <x v="1"/>
@@ -7832,15 +7991,15 @@
     <n v="450194"/>
     <x v="1"/>
     <n v="485108"/>
-    <n v="22441400"/>
+    <n v="13952300"/>
   </r>
   <r>
     <x v="1"/>
     <x v="3"/>
     <n v="194"/>
     <x v="0"/>
-    <n v="590"/>
-    <n v="131000"/>
+    <n v="965"/>
+    <n v="129900"/>
   </r>
   <r>
     <x v="1"/>
@@ -7848,15 +8007,15 @@
     <n v="194"/>
     <x v="1"/>
     <n v="491"/>
-    <n v="168900"/>
+    <n v="214900"/>
   </r>
   <r>
     <x v="1"/>
     <x v="4"/>
     <n v="717"/>
     <x v="0"/>
-    <n v="2718"/>
-    <n v="216800"/>
+    <n v="4540"/>
+    <n v="169200"/>
   </r>
   <r>
     <x v="1"/>
@@ -7864,15 +8023,15 @@
     <n v="717"/>
     <x v="1"/>
     <n v="1439"/>
-    <n v="348100"/>
+    <n v="177900"/>
   </r>
   <r>
     <x v="1"/>
     <x v="5"/>
     <n v="112486"/>
     <x v="0"/>
-    <n v="541504"/>
-    <n v="3157700"/>
+    <n v="982006"/>
+    <n v="1720200"/>
   </r>
   <r>
     <x v="1"/>
@@ -7880,15 +8039,15 @@
     <n v="112486"/>
     <x v="1"/>
     <n v="126910"/>
-    <n v="2679600"/>
+    <n v="2184900"/>
   </r>
   <r>
     <x v="1"/>
     <x v="6"/>
     <n v="11244751"/>
     <x v="0"/>
-    <n v="59840404"/>
-    <n v="267353500"/>
+    <n v="110211671"/>
+    <n v="152229900"/>
   </r>
   <r>
     <x v="1"/>
@@ -7896,14 +8055,14 @@
     <n v="11244751"/>
     <x v="1"/>
     <n v="11407621"/>
-    <n v="177443600"/>
+    <n v="199905000"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="100"/>
     <x v="2"/>
-    <n v="300"/>
+    <n v="400"/>
     <m/>
   </r>
   <r>
@@ -7911,7 +8070,7 @@
     <x v="3"/>
     <n v="400"/>
     <x v="2"/>
-    <n v="1200"/>
+    <n v="1600"/>
     <m/>
   </r>
   <r>
@@ -7919,7 +8078,7 @@
     <x v="4"/>
     <n v="1600"/>
     <x v="2"/>
-    <n v="4800"/>
+    <n v="6400"/>
     <m/>
   </r>
   <r>
@@ -7927,7 +8086,7 @@
     <x v="1"/>
     <n v="10000"/>
     <x v="2"/>
-    <n v="30000"/>
+    <n v="40000"/>
     <m/>
   </r>
   <r>
@@ -7935,7 +8094,7 @@
     <x v="5"/>
     <n v="250000"/>
     <x v="2"/>
-    <n v="750000"/>
+    <n v="1000000"/>
     <m/>
   </r>
   <r>
@@ -7943,7 +8102,7 @@
     <x v="2"/>
     <n v="1000000"/>
     <x v="2"/>
-    <n v="3000000"/>
+    <n v="4000000"/>
     <m/>
   </r>
   <r>
@@ -7951,7 +8110,7 @@
     <x v="6"/>
     <n v="25000000"/>
     <x v="2"/>
-    <n v="75000000"/>
+    <n v="100000000"/>
     <m/>
   </r>
   <r>
@@ -7959,7 +8118,7 @@
     <x v="0"/>
     <n v="51"/>
     <x v="2"/>
-    <n v="202"/>
+    <n v="400"/>
     <m/>
   </r>
   <r>
@@ -7967,7 +8126,7 @@
     <x v="3"/>
     <n v="194"/>
     <x v="2"/>
-    <n v="788"/>
+    <n v="1600"/>
     <m/>
   </r>
   <r>
@@ -7975,7 +8134,7 @@
     <x v="4"/>
     <n v="717"/>
     <x v="2"/>
-    <n v="3034"/>
+    <n v="6400"/>
     <m/>
   </r>
   <r>
@@ -7983,7 +8142,7 @@
     <x v="1"/>
     <n v="4544"/>
     <x v="2"/>
-    <n v="19088"/>
+    <n v="40000"/>
     <m/>
   </r>
   <r>
@@ -7991,7 +8150,7 @@
     <x v="5"/>
     <n v="112486"/>
     <x v="2"/>
-    <n v="474972"/>
+    <n v="1000000"/>
     <m/>
   </r>
   <r>
@@ -7999,7 +8158,7 @@
     <x v="2"/>
     <n v="450194"/>
     <x v="2"/>
-    <n v="1900388"/>
+    <n v="4000000"/>
     <m/>
   </r>
   <r>
@@ -8007,7 +8166,7 @@
     <x v="6"/>
     <n v="11244751"/>
     <x v="2"/>
-    <n v="47489502"/>
+    <n v="100000000"/>
     <m/>
   </r>
   <r>
@@ -8015,7 +8174,7 @@
     <x v="0"/>
     <n v="100"/>
     <x v="3"/>
-    <n v="133.21928094887363"/>
+    <n v="232.8771237954945"/>
     <m/>
   </r>
   <r>
@@ -8023,7 +8182,7 @@
     <x v="3"/>
     <n v="400"/>
     <x v="3"/>
-    <n v="486.43856189774726"/>
+    <n v="745.75424759098905"/>
     <m/>
   </r>
   <r>
@@ -8031,7 +8190,7 @@
     <x v="4"/>
     <n v="1600"/>
     <x v="3"/>
-    <n v="1812.8771237954945"/>
+    <n v="2451.5084951819781"/>
     <m/>
   </r>
   <r>
@@ -8039,7 +8198,7 @@
     <x v="1"/>
     <n v="10000"/>
     <x v="3"/>
-    <n v="10664.385618977472"/>
+    <n v="12657.54247590989"/>
     <m/>
   </r>
   <r>
@@ -8047,7 +8206,7 @@
     <x v="5"/>
     <n v="250000"/>
     <x v="3"/>
-    <n v="254482.89214233105"/>
+    <n v="267931.56856932415"/>
     <m/>
   </r>
   <r>
@@ -8055,7 +8214,7 @@
     <x v="2"/>
     <n v="1000000"/>
     <x v="3"/>
-    <n v="1009965.7842846621"/>
+    <n v="1039863.1371386483"/>
     <m/>
   </r>
   <r>
@@ -8063,7 +8222,7 @@
     <x v="6"/>
     <n v="25000000"/>
     <x v="3"/>
-    <n v="25061438.561897747"/>
+    <n v="25245754.247590989"/>
     <m/>
   </r>
   <r>
@@ -8071,7 +8230,7 @@
     <x v="0"/>
     <n v="51"/>
     <x v="3"/>
-    <n v="84.219280948873632"/>
+    <n v="164.44850683942991"/>
     <m/>
   </r>
   <r>
@@ -8079,7 +8238,7 @@
     <x v="3"/>
     <n v="194"/>
     <x v="3"/>
-    <n v="280.43856189774726"/>
+    <n v="497.99651368748511"/>
     <m/>
   </r>
   <r>
@@ -8087,7 +8246,7 @@
     <x v="4"/>
     <n v="717"/>
     <x v="3"/>
-    <n v="929.87712379549453"/>
+    <n v="1475.8663446961523"/>
     <m/>
   </r>
   <r>
@@ -8095,7 +8254,7 @@
     <x v="1"/>
     <n v="4544"/>
     <x v="3"/>
-    <n v="5208.3856189774724"/>
+    <n v="6973.9494239009364"/>
     <m/>
   </r>
   <r>
@@ -8103,7 +8262,7 @@
     <x v="5"/>
     <n v="112486"/>
     <x v="3"/>
-    <n v="116968.89214233104"/>
+    <n v="129265.38592932424"/>
     <m/>
   </r>
   <r>
@@ -8111,7 +8270,7 @@
     <x v="2"/>
     <n v="450194"/>
     <x v="3"/>
-    <n v="460159.78428466211"/>
+    <n v="487754.37460742478"/>
     <m/>
   </r>
   <r>
@@ -8119,14 +8278,14 @@
     <x v="6"/>
     <n v="11244751"/>
     <x v="3"/>
-    <n v="11306189.561897747"/>
+    <n v="11478978.483791253"/>
     <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF3BAF37-11D4-4866-958C-354A73D48CC9}" name="PivotTable21" cacheId="409" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF3BAF37-11D4-4866-958C-354A73D48CC9}" name="PivotTable21" cacheId="170" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A17:F26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
@@ -8329,8 +8488,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E3697355-F798-4EEC-A303-6AD0CE8FC080}" name="PivotTable1" cacheId="409" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="" colHeaderCaption="">
-  <location ref="A3:D12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E3697355-F798-4EEC-A303-6AD0CE8FC080}" name="PivotTable1" cacheId="170" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="" colHeaderCaption="">
+  <location ref="A3:F12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
       <items count="4">
@@ -8356,13 +8515,13 @@
     <pivotField axis="axisCol" showAll="0">
       <items count="9">
         <item x="0"/>
-        <item h="1" x="1"/>
+        <item x="1"/>
         <item h="1" m="1" x="6"/>
         <item h="1" m="1" x="4"/>
         <item h="1" m="1" x="5"/>
         <item h="1" m="1" x="7"/>
         <item x="2"/>
-        <item h="1" x="3"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -8401,12 +8560,18 @@
   <colFields count="1">
     <field x="3"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="5">
     <i>
       <x/>
     </i>
     <i>
+      <x v="1"/>
+    </i>
+    <i>
       <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
     </i>
     <i t="grand">
       <x/>
@@ -8547,7 +8712,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{671E97EB-1ABF-446A-BAEF-C7DF5E760C9E}" name="PivotTable23" cacheId="409" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{671E97EB-1ABF-446A-BAEF-C7DF5E760C9E}" name="PivotTable23" cacheId="170" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A43:D52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
@@ -8735,7 +8900,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E89F3F9-A280-4689-AE55-EFA1BF2722EA}" name="PivotTable22" cacheId="409" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E89F3F9-A280-4689-AE55-EFA1BF2722EA}" name="PivotTable22" cacheId="170" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A30:D39" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
@@ -8900,7 +9065,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFCAB73-DD61-4EAE-99D1-3025614467E3}" name="Table1" displayName="Table1" ref="A1:F57" totalsRowShown="0">
-  <autoFilter ref="A1:F57" xr:uid="{FCFCAB73-DD61-4EAE-99D1-3025614467E3}"/>
+  <autoFilter ref="A1:F57" xr:uid="{FCFCAB73-DD61-4EAE-99D1-3025614467E3}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Array"/>
+        <filter val="Array-theoretically"/>
+        <filter val="Heap-theoretically"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
     <sortCondition ref="A2:A36"/>
     <sortCondition ref="B2:B36" customList="10,100,1000,20,40,500,5000"/>
@@ -9216,167 +9389,221 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70BA030-76AE-4814-9282-180D6DDC2A6D}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
-        <v>50</v>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4">
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
         <v>10</v>
       </c>
-      <c r="B5" s="2">
-        <v>146</v>
-      </c>
-      <c r="C5" s="2">
-        <v>300</v>
-      </c>
-      <c r="D5" s="2">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4">
+      <c r="B5" s="7">
+        <v>222</v>
+      </c>
+      <c r="C5" s="7">
+        <v>213</v>
+      </c>
+      <c r="D5" s="7">
+        <v>400</v>
+      </c>
+      <c r="E5" s="7">
+        <v>232.8771237954945</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1067.8771237954945</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
         <v>20</v>
       </c>
-      <c r="B6" s="2">
-        <v>789</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1200</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1989</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4">
+      <c r="B6" s="7">
+        <v>1253</v>
+      </c>
+      <c r="C6" s="7">
+        <v>740</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1600</v>
+      </c>
+      <c r="E6" s="7">
+        <v>745.75424759098905</v>
+      </c>
+      <c r="F6" s="7">
+        <v>4338.7542475909886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
         <v>40</v>
       </c>
-      <c r="B7" s="2">
-        <v>3217</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4800</v>
-      </c>
-      <c r="D7" s="2">
-        <v>8017</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4">
+      <c r="B7" s="7">
+        <v>5352</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2266</v>
+      </c>
+      <c r="D7" s="7">
+        <v>6400</v>
+      </c>
+      <c r="E7" s="7">
+        <v>2451.5084951819781</v>
+      </c>
+      <c r="F7" s="7">
+        <v>16469.508495181977</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3">
         <v>100</v>
       </c>
-      <c r="B8" s="2">
-        <v>20542</v>
-      </c>
-      <c r="C8" s="2">
-        <v>30000</v>
-      </c>
-      <c r="D8" s="2">
-        <v>50542</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4">
+      <c r="B8" s="7">
+        <v>35277</v>
+      </c>
+      <c r="C8" s="7">
+        <v>12143</v>
+      </c>
+      <c r="D8" s="7">
+        <v>40000</v>
+      </c>
+      <c r="E8" s="7">
+        <v>12657.54247590989</v>
+      </c>
+      <c r="F8" s="7">
+        <v>100077.5424759099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3">
         <v>500</v>
       </c>
-      <c r="B9" s="2">
-        <v>566978</v>
-      </c>
-      <c r="C9" s="2">
-        <v>750000</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1316978</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4">
+      <c r="B9" s="7">
+        <v>1016877</v>
+      </c>
+      <c r="C9" s="7">
+        <v>262592</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="E9" s="7">
+        <v>267931.56856932415</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2547400.568569324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3">
         <v>1000</v>
       </c>
-      <c r="B10" s="2">
-        <v>2267712</v>
-      </c>
-      <c r="C10" s="2">
-        <v>3000000</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5267712</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4">
+      <c r="B10" s="7">
+        <v>4029793</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1027040</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4000000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1039863.1371386483</v>
+      </c>
+      <c r="F10" s="7">
+        <v>10096696.137138648</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3">
         <v>5000</v>
       </c>
-      <c r="B11" s="2">
-        <v>56953404</v>
-      </c>
-      <c r="C11" s="2">
-        <v>75000000</v>
-      </c>
-      <c r="D11" s="2">
-        <v>131953404</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="7">
+        <v>100834480</v>
+      </c>
+      <c r="C11" s="7">
+        <v>25158844</v>
+      </c>
+      <c r="D11" s="7">
+        <v>100000000</v>
+      </c>
+      <c r="E11" s="7">
+        <v>25245754.247590989</v>
+      </c>
+      <c r="F11" s="7">
+        <v>251239078.24759099</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>59812788</v>
-      </c>
-      <c r="C12" s="2">
-        <v>78786300</v>
-      </c>
-      <c r="D12" s="2">
-        <v>138599088</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
+      <c r="B12" s="7">
+        <v>105923254</v>
+      </c>
+      <c r="C12" s="7">
+        <v>26463838</v>
+      </c>
+      <c r="D12" s="7">
+        <v>105048400</v>
+      </c>
+      <c r="E12" s="7">
+        <v>26569636.635641441</v>
+      </c>
+      <c r="F12" s="7">
+        <v>264005128.63564143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B15" t="s">
@@ -9384,15 +9611,15 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B18" t="s">
@@ -9402,177 +9629,177 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>10</v>
       </c>
-      <c r="B19" s="2">
-        <v>136</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="7">
+        <v>198</v>
+      </c>
+      <c r="C19" s="7">
         <v>132</v>
       </c>
-      <c r="D19" s="2">
-        <v>202</v>
-      </c>
-      <c r="E19" s="2">
-        <v>84.219280948873632</v>
-      </c>
-      <c r="F19" s="2">
-        <v>554.21928094887357</v>
+      <c r="D19" s="7">
+        <v>400</v>
+      </c>
+      <c r="E19" s="7">
+        <v>164.44850683942991</v>
+      </c>
+      <c r="F19" s="7">
+        <v>894.44850683942991</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>20</v>
       </c>
-      <c r="B20" s="2">
-        <v>590</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="7">
+        <v>965</v>
+      </c>
+      <c r="C20" s="7">
         <v>491</v>
       </c>
-      <c r="D20" s="2">
-        <v>788</v>
-      </c>
-      <c r="E20" s="2">
-        <v>280.43856189774726</v>
-      </c>
-      <c r="F20" s="2">
-        <v>2149.4385618977471</v>
+      <c r="D20" s="7">
+        <v>1600</v>
+      </c>
+      <c r="E20" s="7">
+        <v>497.99651368748511</v>
+      </c>
+      <c r="F20" s="7">
+        <v>3553.9965136874853</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>40</v>
       </c>
-      <c r="B21" s="2">
-        <v>2718</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="7">
+        <v>4540</v>
+      </c>
+      <c r="C21" s="7">
         <v>1439</v>
       </c>
-      <c r="D21" s="2">
-        <v>3034</v>
-      </c>
-      <c r="E21" s="2">
-        <v>929.87712379549453</v>
-      </c>
-      <c r="F21" s="2">
-        <v>8120.8771237954943</v>
+      <c r="D21" s="7">
+        <v>6400</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1475.8663446961523</v>
+      </c>
+      <c r="F21" s="7">
+        <v>13854.866344696153</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>100</v>
       </c>
-      <c r="B22" s="2">
-        <v>19996</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B22" s="7">
+        <v>35021</v>
+      </c>
+      <c r="C22" s="7">
         <v>6893</v>
       </c>
-      <c r="D22" s="2">
-        <v>19088</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5208.3856189774724</v>
-      </c>
-      <c r="F22" s="2">
-        <v>51185.385618977474</v>
+      <c r="D22" s="7">
+        <v>40000</v>
+      </c>
+      <c r="E22" s="7">
+        <v>6973.9494239009364</v>
+      </c>
+      <c r="F22" s="7">
+        <v>88887.949423900936</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>500</v>
       </c>
-      <c r="B23" s="2">
-        <v>541504</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="B23" s="7">
+        <v>982006</v>
+      </c>
+      <c r="C23" s="7">
         <v>126910</v>
       </c>
-      <c r="D23" s="2">
-        <v>474972</v>
-      </c>
-      <c r="E23" s="2">
-        <v>116968.89214233104</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1260354.892142331</v>
+      <c r="D23" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="E23" s="7">
+        <v>129265.38592932424</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2238181.3859293242</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>1000</v>
       </c>
-      <c r="B24" s="2">
-        <v>2282587</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="B24" s="7">
+        <v>4190113</v>
+      </c>
+      <c r="C24" s="7">
         <v>485108</v>
       </c>
-      <c r="D24" s="2">
-        <v>1900388</v>
-      </c>
-      <c r="E24" s="2">
-        <v>460159.78428466211</v>
-      </c>
-      <c r="F24" s="2">
-        <v>5128242.7842846625</v>
+      <c r="D24" s="7">
+        <v>4000000</v>
+      </c>
+      <c r="E24" s="7">
+        <v>487754.37460742478</v>
+      </c>
+      <c r="F24" s="7">
+        <v>9162975.3746074252</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>5000</v>
       </c>
-      <c r="B25" s="2">
-        <v>59840404</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B25" s="7">
+        <v>110211671</v>
+      </c>
+      <c r="C25" s="7">
         <v>11407621</v>
       </c>
-      <c r="D25" s="2">
-        <v>47489502</v>
-      </c>
-      <c r="E25" s="2">
-        <v>11306189.561897747</v>
-      </c>
-      <c r="F25" s="2">
-        <v>130043716.56189775</v>
+      <c r="D25" s="7">
+        <v>100000000</v>
+      </c>
+      <c r="E25" s="7">
+        <v>11478978.483791253</v>
+      </c>
+      <c r="F25" s="7">
+        <v>233098270.48379126</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="2">
-        <v>62687935</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B26" s="7">
+        <v>115424514</v>
+      </c>
+      <c r="C26" s="7">
         <v>12028594</v>
       </c>
-      <c r="D26" s="2">
-        <v>49887974</v>
-      </c>
-      <c r="E26" s="2">
-        <v>11889821.15891036</v>
-      </c>
-      <c r="F26" s="2">
-        <v>136494324.15891036</v>
+      <c r="D26" s="7">
+        <v>105048400</v>
+      </c>
+      <c r="E26" s="7">
+        <v>12105110.505117126</v>
+      </c>
+      <c r="F26" s="7">
+        <v>244606618.50511715</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B28" t="s">
@@ -9580,15 +9807,15 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B31" t="s">
@@ -9602,119 +9829,119 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>10</v>
       </c>
-      <c r="B32" s="2">
-        <v>13446300</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1594800</v>
-      </c>
-      <c r="D32" s="2">
-        <v>15041100</v>
+      <c r="B32" s="7">
+        <v>12311800</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1774100</v>
+      </c>
+      <c r="D32" s="7">
+        <v>14085900</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>20</v>
       </c>
-      <c r="B33" s="2">
-        <v>370700</v>
-      </c>
-      <c r="C33" s="2">
-        <v>513900</v>
-      </c>
-      <c r="D33" s="2">
-        <v>884600</v>
+      <c r="B33" s="7">
+        <v>257200</v>
+      </c>
+      <c r="C33" s="7">
+        <v>333200</v>
+      </c>
+      <c r="D33" s="7">
+        <v>590400</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>40</v>
       </c>
-      <c r="B34" s="2">
-        <v>277600</v>
-      </c>
-      <c r="C34" s="2">
-        <v>480300</v>
-      </c>
-      <c r="D34" s="2">
-        <v>757900</v>
+      <c r="B34" s="7">
+        <v>257800</v>
+      </c>
+      <c r="C34" s="7">
+        <v>532000</v>
+      </c>
+      <c r="D34" s="7">
+        <v>789800</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>100</v>
       </c>
-      <c r="B35" s="2">
-        <v>3327500</v>
-      </c>
-      <c r="C35" s="2">
-        <v>2649700</v>
-      </c>
-      <c r="D35" s="2">
-        <v>5977200</v>
+      <c r="B35" s="7">
+        <v>2886900</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2933400</v>
+      </c>
+      <c r="D35" s="7">
+        <v>5820300</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>500</v>
       </c>
-      <c r="B36" s="2">
-        <v>3695400</v>
-      </c>
-      <c r="C36" s="2">
-        <v>6060300</v>
-      </c>
-      <c r="D36" s="2">
-        <v>9755700</v>
+      <c r="B36" s="7">
+        <v>3049200</v>
+      </c>
+      <c r="C36" s="7">
+        <v>7701500</v>
+      </c>
+      <c r="D36" s="7">
+        <v>10750700</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>1000</v>
       </c>
-      <c r="B37" s="2">
-        <v>37633000</v>
-      </c>
-      <c r="C37" s="2">
-        <v>54418000</v>
-      </c>
-      <c r="D37" s="2">
-        <v>92051000</v>
+      <c r="B37" s="7">
+        <v>32070100</v>
+      </c>
+      <c r="C37" s="7">
+        <v>64510700</v>
+      </c>
+      <c r="D37" s="7">
+        <v>96580800</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>5000</v>
       </c>
-      <c r="B38" s="2">
-        <v>214762700</v>
-      </c>
-      <c r="C38" s="2">
-        <v>456790100</v>
-      </c>
-      <c r="D38" s="2">
-        <v>671552800</v>
+      <c r="B38" s="7">
+        <v>88495300</v>
+      </c>
+      <c r="C38" s="7">
+        <v>404758400</v>
+      </c>
+      <c r="D38" s="7">
+        <v>493253700</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="2">
-        <v>273513200</v>
-      </c>
-      <c r="C39" s="2">
-        <v>522507100</v>
-      </c>
-      <c r="D39" s="2">
-        <v>796020300</v>
+      <c r="B39" s="7">
+        <v>139328300</v>
+      </c>
+      <c r="C39" s="7">
+        <v>482543300</v>
+      </c>
+      <c r="D39" s="7">
+        <v>621871600</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
@@ -9722,15 +9949,15 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B44" t="s">
@@ -9744,115 +9971,115 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>10</v>
       </c>
-      <c r="B45" s="2">
-        <v>222900</v>
-      </c>
-      <c r="C45" s="2">
-        <v>229200</v>
-      </c>
-      <c r="D45" s="2">
-        <v>452100</v>
+      <c r="B45" s="7">
+        <v>215400</v>
+      </c>
+      <c r="C45" s="7">
+        <v>255400</v>
+      </c>
+      <c r="D45" s="7">
+        <v>470800</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>20</v>
       </c>
-      <c r="B46" s="2">
-        <v>131000</v>
-      </c>
-      <c r="C46" s="2">
-        <v>168900</v>
-      </c>
-      <c r="D46" s="2">
-        <v>299900</v>
+      <c r="B46" s="7">
+        <v>129900</v>
+      </c>
+      <c r="C46" s="7">
+        <v>214900</v>
+      </c>
+      <c r="D46" s="7">
+        <v>344800</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>40</v>
       </c>
-      <c r="B47" s="2">
-        <v>216800</v>
-      </c>
-      <c r="C47" s="2">
-        <v>348100</v>
-      </c>
-      <c r="D47" s="2">
-        <v>564900</v>
+      <c r="B47" s="7">
+        <v>169200</v>
+      </c>
+      <c r="C47" s="7">
+        <v>177900</v>
+      </c>
+      <c r="D47" s="7">
+        <v>347100</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>100</v>
       </c>
-      <c r="B48" s="2">
-        <v>955900</v>
-      </c>
-      <c r="C48" s="2">
-        <v>790100</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1746000</v>
+      <c r="B48" s="7">
+        <v>485200</v>
+      </c>
+      <c r="C48" s="7">
+        <v>772300</v>
+      </c>
+      <c r="D48" s="7">
+        <v>1257500</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>500</v>
       </c>
-      <c r="B49" s="2">
-        <v>3157700</v>
-      </c>
-      <c r="C49" s="2">
-        <v>2679600</v>
-      </c>
-      <c r="D49" s="2">
-        <v>5837300</v>
+      <c r="B49" s="7">
+        <v>1720200</v>
+      </c>
+      <c r="C49" s="7">
+        <v>2184900</v>
+      </c>
+      <c r="D49" s="7">
+        <v>3905100</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>1000</v>
       </c>
-      <c r="B50" s="2">
-        <v>14185300</v>
-      </c>
-      <c r="C50" s="2">
-        <v>22441400</v>
-      </c>
-      <c r="D50" s="2">
-        <v>36626700</v>
+      <c r="B50" s="7">
+        <v>6194100</v>
+      </c>
+      <c r="C50" s="7">
+        <v>13952300</v>
+      </c>
+      <c r="D50" s="7">
+        <v>20146400</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>5000</v>
       </c>
-      <c r="B51" s="2">
-        <v>267353500</v>
-      </c>
-      <c r="C51" s="2">
-        <v>177443600</v>
-      </c>
-      <c r="D51" s="2">
-        <v>444797100</v>
+      <c r="B51" s="7">
+        <v>152229900</v>
+      </c>
+      <c r="C51" s="7">
+        <v>199905000</v>
+      </c>
+      <c r="D51" s="7">
+        <v>352134900</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B52" s="2">
-        <v>286223100</v>
-      </c>
-      <c r="C52" s="2">
-        <v>204100900</v>
-      </c>
-      <c r="D52" s="2">
-        <v>490324000</v>
+      <c r="B52" s="7">
+        <v>161143900</v>
+      </c>
+      <c r="C52" s="7">
+        <v>217462700</v>
+      </c>
+      <c r="D52" s="7">
+        <v>378606600</v>
       </c>
     </row>
   </sheetData>
@@ -9866,8 +10093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D27330-9C12-4449-A4B6-F9FBB001D6A8}">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9881,7 +10108,7 @@
     <col min="16" max="16" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -9901,7 +10128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -9915,14 +10142,22 @@
       <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
-        <v>146</v>
-      </c>
-      <c r="F2" s="2">
-        <v>13446300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2" s="7">
+        <v>222</v>
+      </c>
+      <c r="F2" s="7">
+        <v>12311800</v>
+      </c>
+      <c r="H2" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>122</v>
+      </c>
+      <c r="I2">
+        <f>H2/Table1[[#This Row],[Edges]]</f>
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9936,14 +10171,22 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="7">
         <v>213</v>
       </c>
-      <c r="F3" s="2">
-        <v>1594800</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="7">
+        <v>1774100</v>
+      </c>
+      <c r="H3" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>113</v>
+      </c>
+      <c r="I3">
+        <f>H3/Table1[[#This Row],[Edges]]</f>
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -9957,14 +10200,22 @@
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2">
-        <v>20542</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3327500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" s="7">
+        <v>35277</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2886900</v>
+      </c>
+      <c r="H4" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>25277</v>
+      </c>
+      <c r="I4">
+        <f>H4/Table1[[#This Row],[Edges]]</f>
+        <v>2.5276999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" hidden="1">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -9978,14 +10229,22 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="7">
         <v>12143</v>
       </c>
-      <c r="F5" s="2">
-        <v>2649700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" s="7">
+        <v>2933400</v>
+      </c>
+      <c r="H5" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>2143</v>
+      </c>
+      <c r="I5">
+        <f>H5/Table1[[#This Row],[Edges]]</f>
+        <v>0.21429999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -9999,14 +10258,22 @@
       <c r="D6" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
-        <v>2267712</v>
-      </c>
-      <c r="F6" s="2">
-        <v>37633000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="7">
+        <v>4029793</v>
+      </c>
+      <c r="F6" s="7">
+        <v>32070100</v>
+      </c>
+      <c r="H6" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>3029793</v>
+      </c>
+      <c r="I6">
+        <f>H6/Table1[[#This Row],[Edges]]</f>
+        <v>3.0297930000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" hidden="1">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -10020,14 +10287,22 @@
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="7">
         <v>1027040</v>
       </c>
-      <c r="F7" s="2">
-        <v>54418000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" s="7">
+        <v>64510700</v>
+      </c>
+      <c r="H7" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>27040</v>
+      </c>
+      <c r="I7">
+        <f>H7/Table1[[#This Row],[Edges]]</f>
+        <v>2.7040000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -10041,14 +10316,22 @@
       <c r="D8" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="2">
-        <v>789</v>
-      </c>
-      <c r="F8" s="2">
-        <v>370700</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" s="7">
+        <v>1253</v>
+      </c>
+      <c r="F8" s="7">
+        <v>257200</v>
+      </c>
+      <c r="H8" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>853</v>
+      </c>
+      <c r="I8">
+        <f>H8/Table1[[#This Row],[Edges]]</f>
+        <v>2.1324999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -10062,14 +10345,22 @@
       <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="7">
         <v>740</v>
       </c>
-      <c r="F9" s="2">
-        <v>513900</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="7">
+        <v>333200</v>
+      </c>
+      <c r="H9" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>340</v>
+      </c>
+      <c r="I9">
+        <f>H9/Table1[[#This Row],[Edges]]</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -10083,14 +10374,22 @@
       <c r="D10" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="2">
-        <v>3217</v>
-      </c>
-      <c r="F10" s="2">
-        <v>277600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" s="7">
+        <v>5352</v>
+      </c>
+      <c r="F10" s="7">
+        <v>257800</v>
+      </c>
+      <c r="H10" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>3752</v>
+      </c>
+      <c r="I10">
+        <f>H10/Table1[[#This Row],[Edges]]</f>
+        <v>2.3450000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -10104,14 +10403,22 @@
       <c r="D11" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="7">
         <v>2266</v>
       </c>
-      <c r="F11" s="2">
-        <v>480300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="7">
+        <v>532000</v>
+      </c>
+      <c r="H11" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>666</v>
+      </c>
+      <c r="I11">
+        <f>H11/Table1[[#This Row],[Edges]]</f>
+        <v>0.41625000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -10125,14 +10432,22 @@
       <c r="D12" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="2">
-        <v>566978</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3695400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" s="7">
+        <v>1016877</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3049200</v>
+      </c>
+      <c r="H12" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>766877</v>
+      </c>
+      <c r="I12">
+        <f>H12/Table1[[#This Row],[Edges]]</f>
+        <v>3.0675080000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -10146,14 +10461,22 @@
       <c r="D13" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="7">
         <v>262592</v>
       </c>
-      <c r="F13" s="2">
-        <v>6060300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="F13" s="7">
+        <v>7701500</v>
+      </c>
+      <c r="H13" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>12592</v>
+      </c>
+      <c r="I13">
+        <f>H13/Table1[[#This Row],[Edges]]</f>
+        <v>5.0368000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -10167,14 +10490,22 @@
       <c r="D14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="2">
-        <v>56953404</v>
-      </c>
-      <c r="F14" s="2">
-        <v>214762700</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" s="7">
+        <v>100834480</v>
+      </c>
+      <c r="F14" s="7">
+        <v>88495300</v>
+      </c>
+      <c r="H14" s="11">
+        <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
+        <v>75834480</v>
+      </c>
+      <c r="I14">
+        <f>H14/Table1[[#This Row],[Edges]]</f>
+        <v>3.0333792000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -10188,14 +10519,14 @@
       <c r="D15" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="7">
         <v>25158844</v>
       </c>
-      <c r="F15" s="2">
-        <v>456790100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15" s="7">
+        <v>404758400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -10208,14 +10539,14 @@
       <c r="D16" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="2">
-        <v>136</v>
-      </c>
-      <c r="F16" s="2">
-        <v>222900</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="E16" s="7">
+        <v>198</v>
+      </c>
+      <c r="F16" s="7">
+        <v>215400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" hidden="1">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -10228,14 +10559,14 @@
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="7">
         <v>132</v>
       </c>
-      <c r="F17" s="2">
-        <v>229200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="F17" s="7">
+        <v>255400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -10248,14 +10579,14 @@
       <c r="D18" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="2">
-        <v>19996</v>
-      </c>
-      <c r="F18" s="2">
-        <v>955900</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="E18" s="7">
+        <v>35021</v>
+      </c>
+      <c r="F18" s="7">
+        <v>485200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -10268,14 +10599,14 @@
       <c r="D19" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="7">
         <v>6893</v>
       </c>
-      <c r="F19" s="2">
-        <v>790100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="F19" s="7">
+        <v>772300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -10288,14 +10619,14 @@
       <c r="D20" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="2">
-        <v>2282587</v>
-      </c>
-      <c r="F20" s="2">
-        <v>14185300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="E20" s="7">
+        <v>4190113</v>
+      </c>
+      <c r="F20" s="7">
+        <v>6194100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -10308,14 +10639,14 @@
       <c r="D21" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="7">
         <v>485108</v>
       </c>
-      <c r="F21" s="2">
-        <v>22441400</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="F21" s="7">
+        <v>13952300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -10328,14 +10659,14 @@
       <c r="D22" t="s">
         <v>0</v>
       </c>
-      <c r="E22" s="2">
-        <v>590</v>
-      </c>
-      <c r="F22" s="2">
-        <v>131000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="E22" s="7">
+        <v>965</v>
+      </c>
+      <c r="F22" s="7">
+        <v>129900</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -10348,14 +10679,14 @@
       <c r="D23" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="7">
         <v>491</v>
       </c>
-      <c r="F23" s="2">
-        <v>168900</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="F23" s="7">
+        <v>214900</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -10368,14 +10699,14 @@
       <c r="D24" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="2">
-        <v>2718</v>
-      </c>
-      <c r="F24" s="2">
-        <v>216800</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="E24" s="7">
+        <v>4540</v>
+      </c>
+      <c r="F24" s="7">
+        <v>169200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -10388,14 +10719,14 @@
       <c r="D25" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="7">
         <v>1439</v>
       </c>
-      <c r="F25" s="2">
-        <v>348100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="F25" s="7">
+        <v>177900</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -10408,14 +10739,14 @@
       <c r="D26" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="2">
-        <v>541504</v>
-      </c>
-      <c r="F26" s="2">
-        <v>3157700</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="E26" s="7">
+        <v>982006</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1720200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -10428,14 +10759,14 @@
       <c r="D27" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="7">
         <v>126910</v>
       </c>
-      <c r="F27" s="2">
-        <v>2679600</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="F27" s="7">
+        <v>2184900</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -10448,14 +10779,14 @@
       <c r="D28" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="2">
-        <v>59840404</v>
-      </c>
-      <c r="F28" s="2">
-        <v>267353500</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="E28" s="7">
+        <v>110211671</v>
+      </c>
+      <c r="F28" s="7">
+        <v>152229900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -10468,14 +10799,14 @@
       <c r="D29" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="7">
         <v>11407621</v>
       </c>
-      <c r="F29" s="2">
-        <v>177443600</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="F29" s="7">
+        <v>199905000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -10486,14 +10817,18 @@
         <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E30">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>400</v>
+      </c>
+      <c r="H30">
+        <f>LOG(2,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -10504,14 +10839,14 @@
         <v>400</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E31">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -10522,11 +10857,11 @@
         <v>1600</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E32">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>4800</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>6400</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -10540,11 +10875,11 @@
         <v>10000</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E33">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>30000</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>40000</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -10558,11 +10893,11 @@
         <v>250000</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E34">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>750000</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>1000000</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -10576,11 +10911,11 @@
         <v>1000000</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E35">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>3000000</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>4000000</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -10594,11 +10929,11 @@
         <v>25000000</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E36">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>75000000</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>100000000</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -10612,11 +10947,11 @@
         <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E37">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>202</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -10630,11 +10965,11 @@
         <v>194</v>
       </c>
       <c r="D38" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E38">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>788</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>1600</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -10648,11 +10983,11 @@
         <v>717</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E39">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>3034</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>6400</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -10666,11 +11001,11 @@
         <v>4544</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E40">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>19088</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>40000</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -10684,11 +11019,11 @@
         <v>112486</v>
       </c>
       <c r="D41" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E41">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>474972</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>1000000</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -10702,11 +11037,11 @@
         <v>450194</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E42">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>1900388</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>4000000</v>
       </c>
       <c r="J42" t="s">
         <v>15</v>
@@ -10723,17 +11058,17 @@
         <v>11244751</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E43">
-        <f>2*Table1[[#This Row],[Edges]]+POWER(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>47489502</v>
+        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <v>100000000</v>
       </c>
       <c r="J43" t="s">
         <v>16</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="Q43" t="str" cm="1">
         <f t="array" ref="Q43:U43">_xlfn.TEXTSPLIT(P43,",")</f>
@@ -10746,10 +11081,10 @@
         <v>Array</v>
       </c>
       <c r="T43" t="str">
-        <v>146</v>
+        <v>222</v>
       </c>
       <c r="U43" t="str">
-        <v>13446300</v>
+        <v>12311800</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -10763,13 +11098,13 @@
         <v>100</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>133.21928094887363</v>
-      </c>
-      <c r="F44" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E44" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>232.8771237954945</v>
+      </c>
+      <c r="F44" s="5"/>
       <c r="I44" t="s">
         <v>18</v>
       </c>
@@ -10777,7 +11112,7 @@
         <v>17</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="Q44" t="str" cm="1">
         <f t="array" ref="Q44:U44">_xlfn.TEXTSPLIT(P44,",")</f>
@@ -10793,7 +11128,7 @@
         <v>213</v>
       </c>
       <c r="U44" t="str">
-        <v>1594800</v>
+        <v>1774100</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -10807,15 +11142,15 @@
         <v>400</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
-      </c>
-      <c r="E45" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>486.43856189774726</v>
-      </c>
-      <c r="F45" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E45" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>745.75424759098905</v>
+      </c>
+      <c r="F45" s="5"/>
       <c r="P45" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Q45" t="str" cm="1">
         <f t="array" ref="Q45:U45">_xlfn.TEXTSPLIT(P45,",")</f>
@@ -10828,10 +11163,10 @@
         <v>Array</v>
       </c>
       <c r="T45" t="str">
-        <v>20542</v>
+        <v>35277</v>
       </c>
       <c r="U45" t="str">
-        <v>3327500</v>
+        <v>2886900</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -10845,15 +11180,15 @@
         <v>1600</v>
       </c>
       <c r="D46" t="s">
-        <v>49</v>
-      </c>
-      <c r="E46" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>1812.8771237954945</v>
-      </c>
-      <c r="F46" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E46" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>2451.5084951819781</v>
+      </c>
+      <c r="F46" s="5"/>
       <c r="P46" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="Q46" t="str" cm="1">
         <f t="array" ref="Q46:U46">_xlfn.TEXTSPLIT(P46,",")</f>
@@ -10869,7 +11204,7 @@
         <v>12143</v>
       </c>
       <c r="U46" t="str">
-        <v>2649700</v>
+        <v>2933400</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -10883,15 +11218,15 @@
         <v>10000</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>10664.385618977472</v>
-      </c>
-      <c r="F47" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E47" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>12657.54247590989</v>
+      </c>
+      <c r="F47" s="5"/>
       <c r="P47" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="Q47" t="str" cm="1">
         <f t="array" ref="Q47:U47">_xlfn.TEXTSPLIT(P47,",")</f>
@@ -10904,10 +11239,10 @@
         <v>Array</v>
       </c>
       <c r="T47" t="str">
-        <v>2267712</v>
+        <v>4029793</v>
       </c>
       <c r="U47" t="str">
-        <v>37633000</v>
+        <v>32070100</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -10921,18 +11256,18 @@
         <v>250000</v>
       </c>
       <c r="D48" t="s">
-        <v>49</v>
-      </c>
-      <c r="E48" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>254482.89214233105</v>
-      </c>
-      <c r="F48" s="6"/>
-      <c r="I48" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>267931.56856932415</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="I48" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q48" t="str" cm="1">
         <f t="array" ref="Q48:U48">_xlfn.TEXTSPLIT(P48,",")</f>
@@ -10948,7 +11283,7 @@
         <v>1027040</v>
       </c>
       <c r="U48" t="str">
-        <v>54418000</v>
+        <v>64510700</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -10962,15 +11297,15 @@
         <v>1000000</v>
       </c>
       <c r="D49" t="s">
-        <v>49</v>
-      </c>
-      <c r="E49" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>1009965.7842846621</v>
-      </c>
-      <c r="F49" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E49" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>1039863.1371386483</v>
+      </c>
+      <c r="F49" s="5"/>
       <c r="P49" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Q49" t="str" cm="1">
         <f t="array" ref="Q49:U49">_xlfn.TEXTSPLIT(P49,",")</f>
@@ -10983,10 +11318,10 @@
         <v>Array</v>
       </c>
       <c r="T49" t="str">
-        <v>789</v>
+        <v>1253</v>
       </c>
       <c r="U49" t="str">
-        <v>370700</v>
+        <v>257200</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -11000,15 +11335,15 @@
         <v>25000000</v>
       </c>
       <c r="D50" t="s">
-        <v>49</v>
-      </c>
-      <c r="E50" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>25061438.561897747</v>
-      </c>
-      <c r="F50" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E50" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>25245754.247590989</v>
+      </c>
+      <c r="F50" s="5"/>
       <c r="P50" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="Q50" t="str" cm="1">
         <f t="array" ref="Q50:U50">_xlfn.TEXTSPLIT(P50,",")</f>
@@ -11024,7 +11359,7 @@
         <v>740</v>
       </c>
       <c r="U50" t="str">
-        <v>513900</v>
+        <v>333200</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -11038,16 +11373,16 @@
         <v>51</v>
       </c>
       <c r="D51" t="s">
-        <v>49</v>
-      </c>
-      <c r="E51" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>84.219280948873632</v>
-      </c>
-      <c r="F51" s="6"/>
-      <c r="H51" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="E51" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>164.44850683942991</v>
+      </c>
+      <c r="F51" s="5"/>
+      <c r="H51" s="6"/>
       <c r="P51" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q51" t="str" cm="1">
         <f t="array" ref="Q51:U51">_xlfn.TEXTSPLIT(P51,",")</f>
@@ -11060,10 +11395,10 @@
         <v>Array</v>
       </c>
       <c r="T51" t="str">
-        <v>3217</v>
+        <v>5352</v>
       </c>
       <c r="U51" t="str">
-        <v>277600</v>
+        <v>257800</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -11077,15 +11412,15 @@
         <v>194</v>
       </c>
       <c r="D52" t="s">
-        <v>49</v>
-      </c>
-      <c r="E52" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>280.43856189774726</v>
-      </c>
-      <c r="F52" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E52" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>497.99651368748511</v>
+      </c>
+      <c r="F52" s="5"/>
       <c r="P52" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Q52" t="str" cm="1">
         <f t="array" ref="Q52:U52">_xlfn.TEXTSPLIT(P52,",")</f>
@@ -11101,7 +11436,7 @@
         <v>2266</v>
       </c>
       <c r="U52" t="str">
-        <v>480300</v>
+        <v>532000</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -11115,15 +11450,15 @@
         <v>717</v>
       </c>
       <c r="D53" t="s">
-        <v>49</v>
-      </c>
-      <c r="E53" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>929.87712379549453</v>
-      </c>
-      <c r="F53" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E53" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>1475.8663446961523</v>
+      </c>
+      <c r="F53" s="5"/>
       <c r="P53" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q53" t="str" cm="1">
         <f t="array" ref="Q53:U53">_xlfn.TEXTSPLIT(P53,",")</f>
@@ -11136,10 +11471,10 @@
         <v>Array</v>
       </c>
       <c r="T53" t="str">
-        <v>566978</v>
+        <v>1016877</v>
       </c>
       <c r="U53" t="str">
-        <v>3695400</v>
+        <v>3049200</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -11153,15 +11488,15 @@
         <v>4544</v>
       </c>
       <c r="D54" t="s">
-        <v>49</v>
-      </c>
-      <c r="E54" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>5208.3856189774724</v>
-      </c>
-      <c r="F54" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E54" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>6973.9494239009364</v>
+      </c>
+      <c r="F54" s="5"/>
       <c r="P54" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Q54" t="str" cm="1">
         <f t="array" ref="Q54:U54">_xlfn.TEXTSPLIT(P54,",")</f>
@@ -11177,7 +11512,7 @@
         <v>262592</v>
       </c>
       <c r="U54" t="str">
-        <v>6060300</v>
+        <v>7701500</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -11191,15 +11526,15 @@
         <v>112486</v>
       </c>
       <c r="D55" t="s">
-        <v>49</v>
-      </c>
-      <c r="E55" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>116968.89214233104</v>
-      </c>
-      <c r="F55" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E55" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>129265.38592932424</v>
+      </c>
+      <c r="F55" s="5"/>
       <c r="P55" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="Q55" t="str" cm="1">
         <f t="array" ref="Q55:U55">_xlfn.TEXTSPLIT(P55,",")</f>
@@ -11212,10 +11547,10 @@
         <v>Array</v>
       </c>
       <c r="T55" t="str">
-        <v>56953404</v>
+        <v>100834480</v>
       </c>
       <c r="U55" t="str">
-        <v>214762700</v>
+        <v>88495300</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -11229,15 +11564,15 @@
         <v>450194</v>
       </c>
       <c r="D56" t="s">
-        <v>49</v>
-      </c>
-      <c r="E56" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>460159.78428466211</v>
-      </c>
-      <c r="F56" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E56" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>487754.37460742478</v>
+      </c>
+      <c r="F56" s="5"/>
       <c r="P56" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q56" t="str" cm="1">
         <f t="array" ref="Q56:U56">_xlfn.TEXTSPLIT(P56,",")</f>
@@ -11253,7 +11588,7 @@
         <v>25158844</v>
       </c>
       <c r="U56" t="str">
-        <v>456790100</v>
+        <v>404758400</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -11267,15 +11602,15 @@
         <v>11244751</v>
       </c>
       <c r="D57" t="s">
-        <v>49</v>
-      </c>
-      <c r="E57" s="6">
-        <f>(Table1[[#This Row],[Edges]])+(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2)</f>
-        <v>11306189.561897747</v>
-      </c>
-      <c r="F57" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E57" s="5">
+        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
+        <v>11478978.483791253</v>
+      </c>
+      <c r="F57" s="5"/>
       <c r="P57" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Q57" t="str" cm="1">
         <f t="array" ref="Q57:U57">_xlfn.TEXTSPLIT(P57,",")</f>
@@ -11288,15 +11623,15 @@
         <v>Array</v>
       </c>
       <c r="T57" t="str">
-        <v>136</v>
+        <v>198</v>
       </c>
       <c r="U57" t="str">
-        <v>222900</v>
+        <v>215400</v>
       </c>
     </row>
     <row r="58" spans="1:21">
       <c r="P58" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="Q58" t="str" cm="1">
         <f t="array" ref="Q58:U58">_xlfn.TEXTSPLIT(P58,",")</f>
@@ -11312,12 +11647,12 @@
         <v>132</v>
       </c>
       <c r="U58" t="str">
-        <v>229200</v>
+        <v>255400</v>
       </c>
     </row>
     <row r="59" spans="1:21">
       <c r="P59" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="Q59" t="str" cm="1">
         <f t="array" ref="Q59:U59">_xlfn.TEXTSPLIT(P59,",")</f>
@@ -11330,15 +11665,15 @@
         <v>Array</v>
       </c>
       <c r="T59" t="str">
-        <v>19996</v>
+        <v>35021</v>
       </c>
       <c r="U59" t="str">
-        <v>955900</v>
+        <v>485200</v>
       </c>
     </row>
     <row r="60" spans="1:21">
       <c r="P60" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="Q60" t="str" cm="1">
         <f t="array" ref="Q60:U60">_xlfn.TEXTSPLIT(P60,",")</f>
@@ -11354,12 +11689,12 @@
         <v>6893</v>
       </c>
       <c r="U60" t="str">
-        <v>790100</v>
+        <v>772300</v>
       </c>
     </row>
     <row r="61" spans="1:21">
       <c r="P61" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Q61" t="str" cm="1">
         <f t="array" ref="Q61:U61">_xlfn.TEXTSPLIT(P61,",")</f>
@@ -11372,15 +11707,15 @@
         <v>Array</v>
       </c>
       <c r="T61" t="str">
-        <v>2282587</v>
+        <v>4190113</v>
       </c>
       <c r="U61" t="str">
-        <v>14185300</v>
+        <v>6194100</v>
       </c>
     </row>
     <row r="62" spans="1:21">
       <c r="P62" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q62" t="str" cm="1">
         <f t="array" ref="Q62:U62">_xlfn.TEXTSPLIT(P62,",")</f>
@@ -11396,12 +11731,12 @@
         <v>485108</v>
       </c>
       <c r="U62" t="str">
-        <v>22441400</v>
+        <v>13952300</v>
       </c>
     </row>
     <row r="63" spans="1:21">
       <c r="P63" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="Q63" t="str" cm="1">
         <f t="array" ref="Q63:U63">_xlfn.TEXTSPLIT(P63,",")</f>
@@ -11414,15 +11749,15 @@
         <v>Array</v>
       </c>
       <c r="T63" t="str">
-        <v>590</v>
+        <v>965</v>
       </c>
       <c r="U63" t="str">
-        <v>131000</v>
+        <v>129900</v>
       </c>
     </row>
     <row r="64" spans="1:21">
       <c r="P64" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="Q64" t="str" cm="1">
         <f t="array" ref="Q64:U64">_xlfn.TEXTSPLIT(P64,",")</f>
@@ -11438,12 +11773,12 @@
         <v>491</v>
       </c>
       <c r="U64" t="str">
-        <v>168900</v>
+        <v>214900</v>
       </c>
     </row>
     <row r="65" spans="16:21">
       <c r="P65" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="Q65" t="str" cm="1">
         <f t="array" ref="Q65:U65">_xlfn.TEXTSPLIT(P65,",")</f>
@@ -11456,15 +11791,15 @@
         <v>Array</v>
       </c>
       <c r="T65" t="str">
-        <v>2718</v>
+        <v>4540</v>
       </c>
       <c r="U65" t="str">
-        <v>216800</v>
+        <v>169200</v>
       </c>
     </row>
     <row r="66" spans="16:21">
       <c r="P66" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="Q66" t="str" cm="1">
         <f t="array" ref="Q66:U66">_xlfn.TEXTSPLIT(P66,",")</f>
@@ -11480,12 +11815,12 @@
         <v>1439</v>
       </c>
       <c r="U66" t="str">
-        <v>348100</v>
+        <v>177900</v>
       </c>
     </row>
     <row r="67" spans="16:21">
       <c r="P67" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="Q67" t="str" cm="1">
         <f t="array" ref="Q67:U67">_xlfn.TEXTSPLIT(P67,",")</f>
@@ -11498,15 +11833,15 @@
         <v>Array</v>
       </c>
       <c r="T67" t="str">
-        <v>541504</v>
+        <v>982006</v>
       </c>
       <c r="U67" t="str">
-        <v>3157700</v>
+        <v>1720200</v>
       </c>
     </row>
     <row r="68" spans="16:21">
       <c r="P68" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="Q68" t="str" cm="1">
         <f t="array" ref="Q68:U68">_xlfn.TEXTSPLIT(P68,",")</f>
@@ -11522,12 +11857,12 @@
         <v>126910</v>
       </c>
       <c r="U68" t="str">
-        <v>2679600</v>
+        <v>2184900</v>
       </c>
     </row>
     <row r="69" spans="16:21">
       <c r="P69" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Q69" t="str" cm="1">
         <f t="array" ref="Q69:U69">_xlfn.TEXTSPLIT(P69,",")</f>
@@ -11540,15 +11875,15 @@
         <v>Array</v>
       </c>
       <c r="T69" t="str">
-        <v>59840404</v>
+        <v>110211671</v>
       </c>
       <c r="U69" t="str">
-        <v>267353500</v>
+        <v>152229900</v>
       </c>
     </row>
     <row r="70" spans="16:21">
       <c r="P70" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q70" t="str" cm="1">
         <f t="array" ref="Q70:U70">_xlfn.TEXTSPLIT(P70,",")</f>
@@ -11564,7 +11899,7 @@
         <v>11407621</v>
       </c>
       <c r="U70" t="str">
-        <v>177443600</v>
+        <v>199905000</v>
       </c>
     </row>
   </sheetData>
@@ -11574,8 +11909,272 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47ACD059-68C1-48DD-91E4-F967774AC188}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A2" s="8">
+        <v>213</v>
+      </c>
+      <c r="B2" s="9">
+        <v>233</v>
+      </c>
+      <c r="C2">
+        <f>100-(A2/B2)*100</f>
+        <v>8.5836909871244558</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A3" s="8">
+        <v>740</v>
+      </c>
+      <c r="B3" s="9">
+        <v>746</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C33" si="0">100-(A3/B3)*100</f>
+        <v>0.80428954423592813</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A4" s="8">
+        <v>2266</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2452</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>7.5856443719412709</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A5" s="8">
+        <v>12143</v>
+      </c>
+      <c r="B5" s="9">
+        <v>12658</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>4.0685732343182224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A6" s="8">
+        <v>262592</v>
+      </c>
+      <c r="B6" s="9">
+        <v>267932</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1.993043010913226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A7" s="8">
+        <v>1027040</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1039863</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1.2331432121346779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A8" s="8">
+        <v>25158844</v>
+      </c>
+      <c r="B8" s="9">
+        <v>25245754</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.344255909330343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A11" s="8">
+        <v>132</v>
+      </c>
+      <c r="B11" s="9">
+        <v>164</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>19.512195121951208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A12" s="8">
+        <v>491</v>
+      </c>
+      <c r="B12" s="9">
+        <v>498</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1.4056224899598391</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A13" s="8">
+        <v>1439</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1476</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>2.5067750677506808</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A14" s="8">
+        <v>6893</v>
+      </c>
+      <c r="B14" s="9">
+        <v>6974</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1.161456839690274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A15" s="8">
+        <v>126910</v>
+      </c>
+      <c r="B15" s="9">
+        <v>129265</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1.8218388581595946</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A16" s="8">
+        <v>485108</v>
+      </c>
+      <c r="B16" s="9">
+        <v>487754</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.54248658135043115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A17" s="8">
+        <v>11407621</v>
+      </c>
+      <c r="B17" s="9">
+        <v>11478978</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.62163199546161252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="12"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="12"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="11"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="12"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="12"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="12"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="12"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="11"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final lab2 with new 80:20 sparse graphs
</commit_message>
<xml_diff>
--- a/Project 2/JavaImpl/Lab2/Analysis2.xlsx
+++ b/Project 2/JavaImpl/Lab2/Analysis2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\NTUwork\SC2001\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC507B0-6E19-4A95-B075-C4B0E76D2905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49A18D6-1DFB-42C9-BCB9-47F313CEEC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{1E6B9D57-98B4-4DC0-9C08-6B8F636F6188}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1E6B9D57-98B4-4DC0-9C08-6B8F636F6188}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualization" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="170" r:id="rId4"/>
+    <pivotCache cacheId="240" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="54">
   <si>
     <t>Array</t>
   </si>
@@ -137,95 +137,104 @@
     <t/>
   </si>
   <si>
-    <t>Dense,10,Array,222,12311800</t>
+    <t>Dense,10,Array,222,1584300</t>
   </si>
   <si>
-    <t>Dense,10,Heap,213,1774100</t>
+    <t>Dense,10,Heap,213,1422200</t>
   </si>
   <si>
-    <t>Dense,100,Array,35277,2886900</t>
+    <t>Dense,100,Array,35277,3336700</t>
   </si>
   <si>
-    <t>Dense,100,Heap,12143,2933400</t>
+    <t>Dense,100,Heap,12143,2892700</t>
   </si>
   <si>
-    <t>Dense,1000,Array,4029793,32070100</t>
+    <t>Dense,1000,Array,4029793,42019700</t>
   </si>
   <si>
-    <t>Dense,1000,Heap,1027040,64510700</t>
+    <t>Dense,1000,Heap,1027040,59701400</t>
   </si>
   <si>
-    <t>Dense,20,Array,1253,257200</t>
+    <t>Dense,20,Array,1253,430100</t>
   </si>
   <si>
-    <t>Dense,20,Heap,740,333200</t>
+    <t>Dense,20,Heap,740,378600</t>
   </si>
   <si>
-    <t>Dense,40,Array,5352,257800</t>
+    <t>Dense,40,Array,5352,246900</t>
   </si>
   <si>
-    <t>Dense,40,Heap,2266,532000</t>
+    <t>Dense,40,Heap,2266,339300</t>
   </si>
   <si>
-    <t>Dense,500,Array,1016877,3049200</t>
+    <t>Dense,500,Array,1016877,4079000</t>
   </si>
   <si>
-    <t>Dense,500,Heap,262592,7701500</t>
+    <t>Dense,500,Heap,262592,7026600</t>
   </si>
   <si>
-    <t>Dense,5000,Array,100834480,88495300</t>
+    <t>Dense,5000,Array,100834480,92804600</t>
   </si>
   <si>
-    <t>Dense,5000,Heap,25158844,404758400</t>
+    <t>Dense,5000,Heap,25158844,506694600</t>
   </si>
   <si>
-    <t>Sparse,10,Array,198,215400</t>
+    <t>Sparse,10,Array,138,206700</t>
   </si>
   <si>
-    <t>Sparse,10,Heap,132,255400</t>
+    <t>Sparse,10,Heap,66,218400</t>
   </si>
   <si>
-    <t>Sparse,100,Array,35021,485200</t>
+    <t>Sparse,100,Array,29361,410000</t>
   </si>
   <si>
-    <t>Sparse,100,Heap,6893,772300</t>
+    <t>Sparse,100,Heap,4291,557200</t>
   </si>
   <si>
-    <t>Sparse,1000,Array,4190113,6194100</t>
+    <t>Sparse,1000,Array,3850228,4938400</t>
   </si>
   <si>
-    <t>Sparse,1000,Heap,485108,13952300</t>
+    <t>Sparse,1000,Heap,228345,9966300</t>
   </si>
   <si>
-    <t>Sparse,20,Array,965,129900</t>
+    <t>Sparse,20,Array,739,167000</t>
   </si>
   <si>
-    <t>Sparse,20,Heap,491,214900</t>
+    <t>Sparse,20,Heap,295,174900</t>
   </si>
   <si>
-    <t>Sparse,40,Array,4540,169200</t>
+    <t>Sparse,40,Array,3776,225300</t>
   </si>
   <si>
-    <t>Sparse,40,Heap,1439,177900</t>
+    <t>Sparse,40,Heap,1106,177400</t>
   </si>
   <si>
-    <t>Sparse,500,Array,982006,1720200</t>
+    <t>Sparse,500,Array,953380,1423600</t>
   </si>
   <si>
-    <t>Sparse,500,Heap,126910,2184900</t>
+    <t>Sparse,500,Heap,64486,1571200</t>
   </si>
   <si>
-    <t>Sparse,5000,Array,110211671,152229900</t>
+    <t>Sparse,5000,Array,107385202,124015400</t>
   </si>
   <si>
-    <t>Sparse,5000,Heap,11407621,199905000</t>
+    <t>Sparse,5000,Heap,5213390,97872700</t>
+  </si>
+  <si>
+    <t>V(2V) + V(2V) = 2v^2 + 2v^2</t>
+  </si>
+  <si>
+    <t>Array-N^2</t>
+  </si>
+  <si>
+    <t>Heap-VLogV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +273,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -279,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -322,11 +339,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -346,8 +372,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1956,6 +1985,118 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="27"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="28"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -2235,7 +2376,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B1DE-4C84-84A5-E0AA04749FFC}"/>
+              <c16:uniqueId val="{00000001-DE7E-48A5-AB37-CFA0C3C4C331}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2302,25 +2443,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>232.8771237954945</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>745.75424759098905</c:v>
+                  <c:v>746</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2451.5084951819781</c:v>
+                  <c:v>2452</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12657.54247590989</c:v>
+                  <c:v>12658</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>267931.56856932415</c:v>
+                  <c:v>267932</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1039863.1371386483</c:v>
+                  <c:v>1039864</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25245754.247590989</c:v>
+                  <c:v>25245755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2328,7 +2469,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B1DE-4C84-84A5-E0AA04749FFC}"/>
+              <c16:uniqueId val="{00000002-DE7E-48A5-AB37-CFA0C3C4C331}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2750,9 +2891,6 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3224,25 +3362,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>198</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>965</c:v>
+                  <c:v>739</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4540</c:v>
+                  <c:v>3776</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35021</c:v>
+                  <c:v>29361</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>982006</c:v>
+                  <c:v>953380</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4190113</c:v>
+                  <c:v>3850228</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>110211671</c:v>
+                  <c:v>107385202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3316,25 +3454,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>132</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>491</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1439</c:v>
+                  <c:v>1106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6893</c:v>
+                  <c:v>4291</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>126910</c:v>
+                  <c:v>64486</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>485108</c:v>
+                  <c:v>228345</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11407621</c:v>
+                  <c:v>5213390</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3435,7 +3573,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-226D-4F0E-8BA5-B4A8B69CF283}"/>
+              <c16:uniqueId val="{00000001-F5F2-473F-97DD-2F84AC62D60A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3502,25 +3640,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>164.44850683942991</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>497.99651368748511</c:v>
+                  <c:v>326</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1475.8663446961523</c:v>
+                  <c:v>1035</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6973.9494239009364</c:v>
+                  <c:v>4155</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>129265.38592932424</c:v>
+                  <c:v>65391</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>487754.37460742478</c:v>
+                  <c:v>234915</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11478978.483791253</c:v>
+                  <c:v>5222437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3528,7 +3666,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-226D-4F0E-8BA5-B4A8B69CF283}"/>
+              <c16:uniqueId val="{00000002-F5F2-473F-97DD-2F84AC62D60A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4253,25 +4391,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12311800</c:v>
+                  <c:v>1584300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>257200</c:v>
+                  <c:v>430100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>257800</c:v>
+                  <c:v>246900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2886900</c:v>
+                  <c:v>3336700</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3049200</c:v>
+                  <c:v>4079000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32070100</c:v>
+                  <c:v>42019700</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88495300</c:v>
+                  <c:v>92804600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4357,25 +4495,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1774100</c:v>
+                  <c:v>1422200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>333200</c:v>
+                  <c:v>378600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>532000</c:v>
+                  <c:v>339300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2933400</c:v>
+                  <c:v>2892700</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7701500</c:v>
+                  <c:v>7026600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64510700</c:v>
+                  <c:v>59701400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>404758400</c:v>
+                  <c:v>506694600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4698,7 +4836,19 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -4754,7 +4904,19 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -5026,7 +5188,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5064,25 +5238,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>215400</c:v>
+                  <c:v>206700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>129900</c:v>
+                  <c:v>167000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>169200</c:v>
+                  <c:v>225300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>485200</c:v>
+                  <c:v>410000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1720200</c:v>
+                  <c:v>1423600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6194100</c:v>
+                  <c:v>4938400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>152229900</c:v>
+                  <c:v>124015400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5118,7 +5292,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -5156,25 +5342,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>255400</c:v>
+                  <c:v>218400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>214900</c:v>
+                  <c:v>174900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>177900</c:v>
+                  <c:v>177400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>772300</c:v>
+                  <c:v>557200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2184900</c:v>
+                  <c:v>1571200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13952300</c:v>
+                  <c:v>9966300</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>199905000</c:v>
+                  <c:v>97872700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5194,6 +5380,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="982108960"/>
         <c:axId val="982105024"/>
@@ -7778,7 +7965,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kiann" refreshedDate="44838.706936574075" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="56" xr:uid="{C1740812-440E-4F27-B842-754C89F7B27F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kiann" refreshedDate="44838.86433611111" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="84" xr:uid="{C1740812-440E-4F27-B842-754C89F7B27F}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -7802,14 +7989,16 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Edges" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="51" maxValue="25000000"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="15" maxValue="25000000"/>
     </cacheField>
     <cacheField name="Implementation" numFmtId="0">
-      <sharedItems containsBlank="1" count="8">
+      <sharedItems containsBlank="1" count="10">
         <s v="Array"/>
         <s v="Heap"/>
         <s v="Array-theoretically"/>
         <s v="Heap-theoretically"/>
+        <s v="Array-N^2"/>
+        <s v="Heap-VLogV"/>
         <m u="1"/>
         <s v="zArray-Worst" u="1"/>
         <s v="Array-Worst" u="1"/>
@@ -7817,10 +8006,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Key Comparison" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="132" maxValue="110211671"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="34" maxValue="107385202"/>
     </cacheField>
     <cacheField name="Time (NS)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="129900" maxValue="404758400"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="167000" maxValue="506694600"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -7832,14 +8021,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="56">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="84">
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="100"/>
     <x v="0"/>
     <n v="222"/>
-    <n v="12311800"/>
+    <n v="1584300"/>
   </r>
   <r>
     <x v="0"/>
@@ -7847,7 +8036,7 @@
     <n v="100"/>
     <x v="1"/>
     <n v="213"/>
-    <n v="1774100"/>
+    <n v="1422200"/>
   </r>
   <r>
     <x v="0"/>
@@ -7855,7 +8044,7 @@
     <n v="10000"/>
     <x v="0"/>
     <n v="35277"/>
-    <n v="2886900"/>
+    <n v="3336700"/>
   </r>
   <r>
     <x v="0"/>
@@ -7863,7 +8052,7 @@
     <n v="10000"/>
     <x v="1"/>
     <n v="12143"/>
-    <n v="2933400"/>
+    <n v="2892700"/>
   </r>
   <r>
     <x v="0"/>
@@ -7871,7 +8060,7 @@
     <n v="1000000"/>
     <x v="0"/>
     <n v="4029793"/>
-    <n v="32070100"/>
+    <n v="42019700"/>
   </r>
   <r>
     <x v="0"/>
@@ -7879,7 +8068,7 @@
     <n v="1000000"/>
     <x v="1"/>
     <n v="1027040"/>
-    <n v="64510700"/>
+    <n v="59701400"/>
   </r>
   <r>
     <x v="0"/>
@@ -7887,7 +8076,7 @@
     <n v="400"/>
     <x v="0"/>
     <n v="1253"/>
-    <n v="257200"/>
+    <n v="430100"/>
   </r>
   <r>
     <x v="0"/>
@@ -7895,7 +8084,7 @@
     <n v="400"/>
     <x v="1"/>
     <n v="740"/>
-    <n v="333200"/>
+    <n v="378600"/>
   </r>
   <r>
     <x v="0"/>
@@ -7903,7 +8092,7 @@
     <n v="1600"/>
     <x v="0"/>
     <n v="5352"/>
-    <n v="257800"/>
+    <n v="246900"/>
   </r>
   <r>
     <x v="0"/>
@@ -7911,7 +8100,7 @@
     <n v="1600"/>
     <x v="1"/>
     <n v="2266"/>
-    <n v="532000"/>
+    <n v="339300"/>
   </r>
   <r>
     <x v="0"/>
@@ -7919,7 +8108,7 @@
     <n v="250000"/>
     <x v="0"/>
     <n v="1016877"/>
-    <n v="3049200"/>
+    <n v="4079000"/>
   </r>
   <r>
     <x v="0"/>
@@ -7927,7 +8116,7 @@
     <n v="250000"/>
     <x v="1"/>
     <n v="262592"/>
-    <n v="7701500"/>
+    <n v="7026600"/>
   </r>
   <r>
     <x v="0"/>
@@ -7935,7 +8124,7 @@
     <n v="25000000"/>
     <x v="0"/>
     <n v="100834480"/>
-    <n v="88495300"/>
+    <n v="92804600"/>
   </r>
   <r>
     <x v="0"/>
@@ -7943,119 +8132,119 @@
     <n v="25000000"/>
     <x v="1"/>
     <n v="25158844"/>
-    <n v="404758400"/>
+    <n v="506694600"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
-    <n v="51"/>
+    <n v="15"/>
     <x v="0"/>
-    <n v="198"/>
-    <n v="215400"/>
+    <n v="138"/>
+    <n v="206700"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
-    <n v="51"/>
+    <n v="15"/>
     <x v="1"/>
-    <n v="132"/>
-    <n v="255400"/>
+    <n v="66"/>
+    <n v="218400"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <n v="4544"/>
+    <n v="1966"/>
     <x v="0"/>
-    <n v="35021"/>
-    <n v="485200"/>
+    <n v="29361"/>
+    <n v="410000"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <n v="4544"/>
+    <n v="1966"/>
     <x v="1"/>
-    <n v="6893"/>
-    <n v="772300"/>
+    <n v="4291"/>
+    <n v="557200"/>
   </r>
   <r>
     <x v="1"/>
     <x v="2"/>
-    <n v="450194"/>
+    <n v="199700"/>
     <x v="0"/>
-    <n v="4190113"/>
-    <n v="6194100"/>
+    <n v="3850228"/>
+    <n v="4938400"/>
   </r>
   <r>
     <x v="1"/>
     <x v="2"/>
-    <n v="450194"/>
+    <n v="199700"/>
     <x v="1"/>
-    <n v="485108"/>
-    <n v="13952300"/>
+    <n v="228345"/>
+    <n v="9966300"/>
   </r>
   <r>
     <x v="1"/>
     <x v="3"/>
-    <n v="194"/>
+    <n v="76"/>
     <x v="0"/>
-    <n v="965"/>
-    <n v="129900"/>
+    <n v="739"/>
+    <n v="167000"/>
   </r>
   <r>
     <x v="1"/>
     <x v="3"/>
-    <n v="194"/>
+    <n v="76"/>
     <x v="1"/>
-    <n v="491"/>
-    <n v="214900"/>
+    <n v="295"/>
+    <n v="174900"/>
   </r>
   <r>
     <x v="1"/>
     <x v="4"/>
-    <n v="717"/>
+    <n v="356"/>
     <x v="0"/>
-    <n v="4540"/>
-    <n v="169200"/>
+    <n v="3776"/>
+    <n v="225300"/>
   </r>
   <r>
     <x v="1"/>
     <x v="4"/>
-    <n v="717"/>
+    <n v="356"/>
     <x v="1"/>
-    <n v="1439"/>
-    <n v="177900"/>
+    <n v="1106"/>
+    <n v="177400"/>
   </r>
   <r>
     <x v="1"/>
     <x v="5"/>
-    <n v="112486"/>
+    <n v="49787"/>
     <x v="0"/>
-    <n v="982006"/>
-    <n v="1720200"/>
+    <n v="953380"/>
+    <n v="1423600"/>
   </r>
   <r>
     <x v="1"/>
     <x v="5"/>
-    <n v="112486"/>
+    <n v="49787"/>
     <x v="1"/>
-    <n v="126910"/>
-    <n v="2184900"/>
+    <n v="64486"/>
+    <n v="1571200"/>
   </r>
   <r>
     <x v="1"/>
     <x v="6"/>
-    <n v="11244751"/>
+    <n v="4999902"/>
     <x v="0"/>
-    <n v="110211671"/>
-    <n v="152229900"/>
+    <n v="107385202"/>
+    <n v="124015400"/>
   </r>
   <r>
     <x v="1"/>
     <x v="6"/>
-    <n v="11244751"/>
+    <n v="4999902"/>
     <x v="1"/>
-    <n v="11407621"/>
-    <n v="199905000"/>
+    <n v="5213390"/>
+    <n v="97872700"/>
   </r>
   <r>
     <x v="0"/>
@@ -8116,7 +8305,7 @@
   <r>
     <x v="1"/>
     <x v="0"/>
-    <n v="51"/>
+    <n v="100"/>
     <x v="2"/>
     <n v="400"/>
     <m/>
@@ -8124,7 +8313,7 @@
   <r>
     <x v="1"/>
     <x v="3"/>
-    <n v="194"/>
+    <n v="400"/>
     <x v="2"/>
     <n v="1600"/>
     <m/>
@@ -8132,7 +8321,7 @@
   <r>
     <x v="1"/>
     <x v="4"/>
-    <n v="717"/>
+    <n v="1600"/>
     <x v="2"/>
     <n v="6400"/>
     <m/>
@@ -8140,7 +8329,7 @@
   <r>
     <x v="1"/>
     <x v="1"/>
-    <n v="4544"/>
+    <n v="10000"/>
     <x v="2"/>
     <n v="40000"/>
     <m/>
@@ -8148,7 +8337,7 @@
   <r>
     <x v="1"/>
     <x v="5"/>
-    <n v="112486"/>
+    <n v="250000"/>
     <x v="2"/>
     <n v="1000000"/>
     <m/>
@@ -8156,7 +8345,7 @@
   <r>
     <x v="1"/>
     <x v="2"/>
-    <n v="450194"/>
+    <n v="1000000"/>
     <x v="2"/>
     <n v="4000000"/>
     <m/>
@@ -8164,7 +8353,7 @@
   <r>
     <x v="1"/>
     <x v="6"/>
-    <n v="11244751"/>
+    <n v="25000000"/>
     <x v="2"/>
     <n v="100000000"/>
     <m/>
@@ -8174,7 +8363,7 @@
     <x v="0"/>
     <n v="100"/>
     <x v="3"/>
-    <n v="232.8771237954945"/>
+    <n v="233"/>
     <m/>
   </r>
   <r>
@@ -8182,7 +8371,7 @@
     <x v="3"/>
     <n v="400"/>
     <x v="3"/>
-    <n v="745.75424759098905"/>
+    <n v="746"/>
     <m/>
   </r>
   <r>
@@ -8190,7 +8379,7 @@
     <x v="4"/>
     <n v="1600"/>
     <x v="3"/>
-    <n v="2451.5084951819781"/>
+    <n v="2452"/>
     <m/>
   </r>
   <r>
@@ -8198,7 +8387,7 @@
     <x v="1"/>
     <n v="10000"/>
     <x v="3"/>
-    <n v="12657.54247590989"/>
+    <n v="12658"/>
     <m/>
   </r>
   <r>
@@ -8206,7 +8395,7 @@
     <x v="5"/>
     <n v="250000"/>
     <x v="3"/>
-    <n v="267931.56856932415"/>
+    <n v="267932"/>
     <m/>
   </r>
   <r>
@@ -8214,7 +8403,7 @@
     <x v="2"/>
     <n v="1000000"/>
     <x v="3"/>
-    <n v="1039863.1371386483"/>
+    <n v="1039864"/>
     <m/>
   </r>
   <r>
@@ -8222,70 +8411,294 @@
     <x v="6"/>
     <n v="25000000"/>
     <x v="3"/>
-    <n v="25245754.247590989"/>
+    <n v="25245755"/>
     <m/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
-    <n v="51"/>
+    <n v="15"/>
     <x v="3"/>
-    <n v="164.44850683942991"/>
+    <n v="94"/>
     <m/>
   </r>
   <r>
     <x v="1"/>
     <x v="3"/>
-    <n v="194"/>
+    <n v="76"/>
     <x v="3"/>
-    <n v="497.99651368748511"/>
+    <n v="326"/>
     <m/>
   </r>
   <r>
     <x v="1"/>
     <x v="4"/>
-    <n v="717"/>
+    <n v="356"/>
     <x v="3"/>
-    <n v="1475.8663446961523"/>
+    <n v="1035"/>
     <m/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <n v="4544"/>
+    <n v="1966"/>
     <x v="3"/>
-    <n v="6973.9494239009364"/>
+    <n v="4155"/>
     <m/>
   </r>
   <r>
     <x v="1"/>
     <x v="5"/>
-    <n v="112486"/>
+    <n v="49787"/>
     <x v="3"/>
-    <n v="129265.38592932424"/>
+    <n v="65391"/>
     <m/>
   </r>
   <r>
     <x v="1"/>
     <x v="2"/>
-    <n v="450194"/>
+    <n v="199700"/>
     <x v="3"/>
-    <n v="487754.37460742478"/>
+    <n v="234915"/>
     <m/>
   </r>
   <r>
     <x v="1"/>
     <x v="6"/>
-    <n v="11244751"/>
+    <n v="4999902"/>
     <x v="3"/>
-    <n v="11478978.483791253"/>
+    <n v="5222437"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="100"/>
+    <x v="4"/>
+    <n v="100"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="400"/>
+    <x v="4"/>
+    <n v="400"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="1600"/>
+    <x v="4"/>
+    <n v="1600"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="10000"/>
+    <x v="4"/>
+    <n v="10000"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="250000"/>
+    <x v="4"/>
+    <n v="250000"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="1000000"/>
+    <x v="4"/>
+    <n v="1000000"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="25000000"/>
+    <x v="4"/>
+    <n v="25000000"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="100"/>
+    <x v="4"/>
+    <n v="100"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="400"/>
+    <x v="4"/>
+    <n v="400"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="1600"/>
+    <x v="4"/>
+    <n v="1600"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="10000"/>
+    <x v="4"/>
+    <n v="10000"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="250000"/>
+    <x v="4"/>
+    <n v="250000"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1000000"/>
+    <x v="4"/>
+    <n v="1000000"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="25000000"/>
+    <x v="4"/>
+    <n v="25000000"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="100"/>
+    <x v="5"/>
+    <n v="34"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="400"/>
+    <x v="5"/>
+    <n v="87"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="1600"/>
+    <x v="5"/>
+    <n v="213"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="10000"/>
+    <x v="5"/>
+    <n v="665"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="250000"/>
+    <x v="5"/>
+    <n v="4483"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="1000000"/>
+    <x v="5"/>
+    <n v="9966"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="25000000"/>
+    <x v="5"/>
+    <n v="61439"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="15"/>
+    <x v="5"/>
+    <n v="34"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="76"/>
+    <x v="5"/>
+    <n v="87"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="356"/>
+    <x v="5"/>
+    <n v="213"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1966"/>
+    <x v="5"/>
+    <n v="665"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="49787"/>
+    <x v="5"/>
+    <n v="4483"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="199700"/>
+    <x v="5"/>
+    <n v="9966"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="4999902"/>
+    <x v="5"/>
+    <n v="61439"/>
     <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF3BAF37-11D4-4866-958C-354A73D48CC9}" name="PivotTable21" cacheId="170" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF3BAF37-11D4-4866-958C-354A73D48CC9}" name="PivotTable21" cacheId="240" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A17:F26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
@@ -8310,15 +8723,17 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="9">
+      <items count="11">
         <item x="0"/>
         <item x="1"/>
-        <item m="1" x="5"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="7"/>
+        <item h="1" m="1" x="7"/>
+        <item h="1" m="1" x="6"/>
+        <item h="1" m="1" x="8"/>
+        <item h="1" m="1" x="9"/>
         <item x="2"/>
         <item x="3"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -8488,7 +8903,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E3697355-F798-4EEC-A303-6AD0CE8FC080}" name="PivotTable1" cacheId="170" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="" colHeaderCaption="">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E3697355-F798-4EEC-A303-6AD0CE8FC080}" name="PivotTable1" cacheId="240" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="" colHeaderCaption="">
   <location ref="A3:F12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
@@ -8513,15 +8928,17 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="9">
+      <items count="11">
         <item x="0"/>
         <item x="1"/>
+        <item h="1" m="1" x="8"/>
         <item h="1" m="1" x="6"/>
-        <item h="1" m="1" x="4"/>
-        <item h="1" m="1" x="5"/>
         <item h="1" m="1" x="7"/>
+        <item h="1" m="1" x="9"/>
         <item x="2"/>
         <item x="3"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -8583,7 +9000,7 @@
   <dataFields count="1">
     <dataField name="Sum of Key Comparison" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="9">
+  <chartFormats count="11">
     <chartFormat chart="0" format="18" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -8698,6 +9115,30 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="0" format="27" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="28" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -8712,7 +9153,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{671E97EB-1ABF-446A-BAEF-C7DF5E760C9E}" name="PivotTable23" cacheId="170" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{671E97EB-1ABF-446A-BAEF-C7DF5E760C9E}" name="PivotTable23" cacheId="240" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A43:D52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
@@ -8737,15 +9178,17 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="9">
+      <items count="11">
         <item x="0"/>
         <item x="1"/>
+        <item h="1" m="1" x="8"/>
         <item h="1" m="1" x="6"/>
-        <item h="1" m="1" x="4"/>
-        <item h="1" m="1" x="5"/>
         <item h="1" m="1" x="7"/>
+        <item h="1" m="1" x="9"/>
         <item h="1" x="2"/>
         <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -8900,7 +9343,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E89F3F9-A280-4689-AE55-EFA1BF2722EA}" name="PivotTable22" cacheId="170" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4E89F3F9-A280-4689-AE55-EFA1BF2722EA}" name="PivotTable22" cacheId="240" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A30:D39" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
@@ -8925,15 +9368,17 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="9">
+      <items count="11">
         <item x="0"/>
         <item x="1"/>
+        <item h="1" m="1" x="8"/>
         <item h="1" m="1" x="6"/>
-        <item h="1" m="1" x="4"/>
-        <item h="1" m="1" x="5"/>
         <item h="1" m="1" x="7"/>
+        <item h="1" m="1" x="9"/>
         <item h="1" x="2"/>
         <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -9064,16 +9509,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFCAB73-DD61-4EAE-99D1-3025614467E3}" name="Table1" displayName="Table1" ref="A1:F57" totalsRowShown="0">
-  <autoFilter ref="A1:F57" xr:uid="{FCFCAB73-DD61-4EAE-99D1-3025614467E3}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Array"/>
-        <filter val="Array-theoretically"/>
-        <filter val="Heap-theoretically"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFCAB73-DD61-4EAE-99D1-3025614467E3}" name="Table1" displayName="Table1" ref="A1:F85" totalsRowShown="0">
+  <autoFilter ref="A1:F85" xr:uid="{FCFCAB73-DD61-4EAE-99D1-3025614467E3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
     <sortCondition ref="A2:A36"/>
     <sortCondition ref="B2:B36" customList="10,100,1000,20,40,500,5000"/>
@@ -9389,21 +9826,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70BA030-76AE-4814-9282-180D6DDC2A6D}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9456,10 +9892,10 @@
         <v>400</v>
       </c>
       <c r="E5" s="7">
-        <v>232.8771237954945</v>
+        <v>233</v>
       </c>
       <c r="F5" s="7">
-        <v>1067.8771237954945</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -9476,10 +9912,10 @@
         <v>1600</v>
       </c>
       <c r="E6" s="7">
-        <v>745.75424759098905</v>
+        <v>746</v>
       </c>
       <c r="F6" s="7">
-        <v>4338.7542475909886</v>
+        <v>4339</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -9496,10 +9932,10 @@
         <v>6400</v>
       </c>
       <c r="E7" s="7">
-        <v>2451.5084951819781</v>
+        <v>2452</v>
       </c>
       <c r="F7" s="7">
-        <v>16469.508495181977</v>
+        <v>16470</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -9516,10 +9952,10 @@
         <v>40000</v>
       </c>
       <c r="E8" s="7">
-        <v>12657.54247590989</v>
+        <v>12658</v>
       </c>
       <c r="F8" s="7">
-        <v>100077.5424759099</v>
+        <v>100078</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -9536,10 +9972,10 @@
         <v>1000000</v>
       </c>
       <c r="E9" s="7">
-        <v>267931.56856932415</v>
+        <v>267932</v>
       </c>
       <c r="F9" s="7">
-        <v>2547400.568569324</v>
+        <v>2547401</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -9556,10 +9992,10 @@
         <v>4000000</v>
       </c>
       <c r="E10" s="7">
-        <v>1039863.1371386483</v>
+        <v>1039864</v>
       </c>
       <c r="F10" s="7">
-        <v>10096696.137138648</v>
+        <v>10096697</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -9576,10 +10012,10 @@
         <v>100000000</v>
       </c>
       <c r="E11" s="7">
-        <v>25245754.247590989</v>
+        <v>25245755</v>
       </c>
       <c r="F11" s="7">
-        <v>251239078.24759099</v>
+        <v>251239079</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -9596,10 +10032,10 @@
         <v>105048400</v>
       </c>
       <c r="E12" s="7">
-        <v>26569636.635641441</v>
+        <v>26569640</v>
       </c>
       <c r="F12" s="7">
-        <v>264005128.63564143</v>
+        <v>264005132</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -9643,19 +10079,19 @@
         <v>10</v>
       </c>
       <c r="B19" s="7">
-        <v>198</v>
+        <v>138</v>
       </c>
       <c r="C19" s="7">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="D19" s="7">
         <v>400</v>
       </c>
       <c r="E19" s="7">
-        <v>164.44850683942991</v>
+        <v>94</v>
       </c>
       <c r="F19" s="7">
-        <v>894.44850683942991</v>
+        <v>698</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -9663,19 +10099,19 @@
         <v>20</v>
       </c>
       <c r="B20" s="7">
-        <v>965</v>
+        <v>739</v>
       </c>
       <c r="C20" s="7">
-        <v>491</v>
+        <v>295</v>
       </c>
       <c r="D20" s="7">
         <v>1600</v>
       </c>
       <c r="E20" s="7">
-        <v>497.99651368748511</v>
+        <v>326</v>
       </c>
       <c r="F20" s="7">
-        <v>3553.9965136874853</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -9683,19 +10119,19 @@
         <v>40</v>
       </c>
       <c r="B21" s="7">
-        <v>4540</v>
+        <v>3776</v>
       </c>
       <c r="C21" s="7">
-        <v>1439</v>
+        <v>1106</v>
       </c>
       <c r="D21" s="7">
         <v>6400</v>
       </c>
       <c r="E21" s="7">
-        <v>1475.8663446961523</v>
+        <v>1035</v>
       </c>
       <c r="F21" s="7">
-        <v>13854.866344696153</v>
+        <v>12317</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -9703,19 +10139,19 @@
         <v>100</v>
       </c>
       <c r="B22" s="7">
-        <v>35021</v>
+        <v>29361</v>
       </c>
       <c r="C22" s="7">
-        <v>6893</v>
+        <v>4291</v>
       </c>
       <c r="D22" s="7">
         <v>40000</v>
       </c>
       <c r="E22" s="7">
-        <v>6973.9494239009364</v>
+        <v>4155</v>
       </c>
       <c r="F22" s="7">
-        <v>88887.949423900936</v>
+        <v>77807</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -9723,19 +10159,19 @@
         <v>500</v>
       </c>
       <c r="B23" s="7">
-        <v>982006</v>
+        <v>953380</v>
       </c>
       <c r="C23" s="7">
-        <v>126910</v>
+        <v>64486</v>
       </c>
       <c r="D23" s="7">
         <v>1000000</v>
       </c>
       <c r="E23" s="7">
-        <v>129265.38592932424</v>
+        <v>65391</v>
       </c>
       <c r="F23" s="7">
-        <v>2238181.3859293242</v>
+        <v>2083257</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -9743,19 +10179,19 @@
         <v>1000</v>
       </c>
       <c r="B24" s="7">
-        <v>4190113</v>
+        <v>3850228</v>
       </c>
       <c r="C24" s="7">
-        <v>485108</v>
+        <v>228345</v>
       </c>
       <c r="D24" s="7">
         <v>4000000</v>
       </c>
       <c r="E24" s="7">
-        <v>487754.37460742478</v>
+        <v>234915</v>
       </c>
       <c r="F24" s="7">
-        <v>9162975.3746074252</v>
+        <v>8313488</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -9763,19 +10199,19 @@
         <v>5000</v>
       </c>
       <c r="B25" s="7">
-        <v>110211671</v>
+        <v>107385202</v>
       </c>
       <c r="C25" s="7">
-        <v>11407621</v>
+        <v>5213390</v>
       </c>
       <c r="D25" s="7">
         <v>100000000</v>
       </c>
       <c r="E25" s="7">
-        <v>11478978.483791253</v>
+        <v>5222437</v>
       </c>
       <c r="F25" s="7">
-        <v>233098270.48379126</v>
+        <v>217821029</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -9783,19 +10219,19 @@
         <v>11</v>
       </c>
       <c r="B26" s="7">
-        <v>115424514</v>
+        <v>112222824</v>
       </c>
       <c r="C26" s="7">
-        <v>12028594</v>
+        <v>5511979</v>
       </c>
       <c r="D26" s="7">
         <v>105048400</v>
       </c>
       <c r="E26" s="7">
-        <v>12105110.505117126</v>
+        <v>5528353</v>
       </c>
       <c r="F26" s="7">
-        <v>244606618.50511715</v>
+        <v>228311556</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -9833,13 +10269,13 @@
         <v>10</v>
       </c>
       <c r="B32" s="7">
-        <v>12311800</v>
+        <v>1584300</v>
       </c>
       <c r="C32" s="7">
-        <v>1774100</v>
+        <v>1422200</v>
       </c>
       <c r="D32" s="7">
-        <v>14085900</v>
+        <v>3006500</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -9847,13 +10283,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="7">
-        <v>257200</v>
+        <v>430100</v>
       </c>
       <c r="C33" s="7">
-        <v>333200</v>
+        <v>378600</v>
       </c>
       <c r="D33" s="7">
-        <v>590400</v>
+        <v>808700</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -9861,13 +10297,13 @@
         <v>40</v>
       </c>
       <c r="B34" s="7">
-        <v>257800</v>
+        <v>246900</v>
       </c>
       <c r="C34" s="7">
-        <v>532000</v>
+        <v>339300</v>
       </c>
       <c r="D34" s="7">
-        <v>789800</v>
+        <v>586200</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -9875,13 +10311,13 @@
         <v>100</v>
       </c>
       <c r="B35" s="7">
-        <v>2886900</v>
+        <v>3336700</v>
       </c>
       <c r="C35" s="7">
-        <v>2933400</v>
+        <v>2892700</v>
       </c>
       <c r="D35" s="7">
-        <v>5820300</v>
+        <v>6229400</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -9889,13 +10325,13 @@
         <v>500</v>
       </c>
       <c r="B36" s="7">
-        <v>3049200</v>
+        <v>4079000</v>
       </c>
       <c r="C36" s="7">
-        <v>7701500</v>
+        <v>7026600</v>
       </c>
       <c r="D36" s="7">
-        <v>10750700</v>
+        <v>11105600</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -9903,13 +10339,13 @@
         <v>1000</v>
       </c>
       <c r="B37" s="7">
-        <v>32070100</v>
+        <v>42019700</v>
       </c>
       <c r="C37" s="7">
-        <v>64510700</v>
+        <v>59701400</v>
       </c>
       <c r="D37" s="7">
-        <v>96580800</v>
+        <v>101721100</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -9917,13 +10353,13 @@
         <v>5000</v>
       </c>
       <c r="B38" s="7">
-        <v>88495300</v>
+        <v>92804600</v>
       </c>
       <c r="C38" s="7">
-        <v>404758400</v>
+        <v>506694600</v>
       </c>
       <c r="D38" s="7">
-        <v>493253700</v>
+        <v>599499200</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -9931,13 +10367,13 @@
         <v>11</v>
       </c>
       <c r="B39" s="7">
-        <v>139328300</v>
+        <v>144501300</v>
       </c>
       <c r="C39" s="7">
-        <v>482543300</v>
+        <v>578455400</v>
       </c>
       <c r="D39" s="7">
-        <v>621871600</v>
+        <v>722956700</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -9975,13 +10411,13 @@
         <v>10</v>
       </c>
       <c r="B45" s="7">
-        <v>215400</v>
+        <v>206700</v>
       </c>
       <c r="C45" s="7">
-        <v>255400</v>
+        <v>218400</v>
       </c>
       <c r="D45" s="7">
-        <v>470800</v>
+        <v>425100</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -9989,13 +10425,13 @@
         <v>20</v>
       </c>
       <c r="B46" s="7">
-        <v>129900</v>
+        <v>167000</v>
       </c>
       <c r="C46" s="7">
-        <v>214900</v>
+        <v>174900</v>
       </c>
       <c r="D46" s="7">
-        <v>344800</v>
+        <v>341900</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -10003,13 +10439,13 @@
         <v>40</v>
       </c>
       <c r="B47" s="7">
-        <v>169200</v>
+        <v>225300</v>
       </c>
       <c r="C47" s="7">
-        <v>177900</v>
+        <v>177400</v>
       </c>
       <c r="D47" s="7">
-        <v>347100</v>
+        <v>402700</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -10017,13 +10453,13 @@
         <v>100</v>
       </c>
       <c r="B48" s="7">
-        <v>485200</v>
+        <v>410000</v>
       </c>
       <c r="C48" s="7">
-        <v>772300</v>
+        <v>557200</v>
       </c>
       <c r="D48" s="7">
-        <v>1257500</v>
+        <v>967200</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -10031,13 +10467,13 @@
         <v>500</v>
       </c>
       <c r="B49" s="7">
-        <v>1720200</v>
+        <v>1423600</v>
       </c>
       <c r="C49" s="7">
-        <v>2184900</v>
+        <v>1571200</v>
       </c>
       <c r="D49" s="7">
-        <v>3905100</v>
+        <v>2994800</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -10045,13 +10481,13 @@
         <v>1000</v>
       </c>
       <c r="B50" s="7">
-        <v>6194100</v>
+        <v>4938400</v>
       </c>
       <c r="C50" s="7">
-        <v>13952300</v>
+        <v>9966300</v>
       </c>
       <c r="D50" s="7">
-        <v>20146400</v>
+        <v>14904700</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -10059,13 +10495,13 @@
         <v>5000</v>
       </c>
       <c r="B51" s="7">
-        <v>152229900</v>
+        <v>124015400</v>
       </c>
       <c r="C51" s="7">
-        <v>199905000</v>
+        <v>97872700</v>
       </c>
       <c r="D51" s="7">
-        <v>352134900</v>
+        <v>221888100</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -10073,13 +10509,13 @@
         <v>11</v>
       </c>
       <c r="B52" s="7">
-        <v>161143900</v>
+        <v>131386400</v>
       </c>
       <c r="C52" s="7">
-        <v>217462700</v>
+        <v>110538100</v>
       </c>
       <c r="D52" s="7">
-        <v>378606600</v>
+        <v>241924500</v>
       </c>
     </row>
   </sheetData>
@@ -10091,10 +10527,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D27330-9C12-4449-A4B6-F9FBB001D6A8}">
-  <dimension ref="A1:U70"/>
+  <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10146,9 +10582,9 @@
         <v>222</v>
       </c>
       <c r="F2" s="7">
-        <v>12311800</v>
-      </c>
-      <c r="H2" s="11">
+        <v>1584300</v>
+      </c>
+      <c r="H2" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>122</v>
       </c>
@@ -10157,7 +10593,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -10175,9 +10611,9 @@
         <v>213</v>
       </c>
       <c r="F3" s="7">
-        <v>1774100</v>
-      </c>
-      <c r="H3" s="11">
+        <v>1422200</v>
+      </c>
+      <c r="H3" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>113</v>
       </c>
@@ -10204,9 +10640,9 @@
         <v>35277</v>
       </c>
       <c r="F4" s="7">
-        <v>2886900</v>
-      </c>
-      <c r="H4" s="11">
+        <v>3336700</v>
+      </c>
+      <c r="H4" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>25277</v>
       </c>
@@ -10215,7 +10651,7 @@
         <v>2.5276999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -10233,9 +10669,9 @@
         <v>12143</v>
       </c>
       <c r="F5" s="7">
-        <v>2933400</v>
-      </c>
-      <c r="H5" s="11">
+        <v>2892700</v>
+      </c>
+      <c r="H5" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>2143</v>
       </c>
@@ -10262,9 +10698,9 @@
         <v>4029793</v>
       </c>
       <c r="F6" s="7">
-        <v>32070100</v>
-      </c>
-      <c r="H6" s="11">
+        <v>42019700</v>
+      </c>
+      <c r="H6" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>3029793</v>
       </c>
@@ -10273,7 +10709,7 @@
         <v>3.0297930000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -10291,9 +10727,9 @@
         <v>1027040</v>
       </c>
       <c r="F7" s="7">
-        <v>64510700</v>
-      </c>
-      <c r="H7" s="11">
+        <v>59701400</v>
+      </c>
+      <c r="H7" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>27040</v>
       </c>
@@ -10320,9 +10756,9 @@
         <v>1253</v>
       </c>
       <c r="F8" s="7">
-        <v>257200</v>
-      </c>
-      <c r="H8" s="11">
+        <v>430100</v>
+      </c>
+      <c r="H8" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>853</v>
       </c>
@@ -10331,7 +10767,7 @@
         <v>2.1324999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -10349,9 +10785,9 @@
         <v>740</v>
       </c>
       <c r="F9" s="7">
-        <v>333200</v>
-      </c>
-      <c r="H9" s="11">
+        <v>378600</v>
+      </c>
+      <c r="H9" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>340</v>
       </c>
@@ -10378,9 +10814,9 @@
         <v>5352</v>
       </c>
       <c r="F10" s="7">
-        <v>257800</v>
-      </c>
-      <c r="H10" s="11">
+        <v>246900</v>
+      </c>
+      <c r="H10" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>3752</v>
       </c>
@@ -10389,7 +10825,7 @@
         <v>2.3450000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -10407,9 +10843,9 @@
         <v>2266</v>
       </c>
       <c r="F11" s="7">
-        <v>532000</v>
-      </c>
-      <c r="H11" s="11">
+        <v>339300</v>
+      </c>
+      <c r="H11" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>666</v>
       </c>
@@ -10436,9 +10872,9 @@
         <v>1016877</v>
       </c>
       <c r="F12" s="7">
-        <v>3049200</v>
-      </c>
-      <c r="H12" s="11">
+        <v>4079000</v>
+      </c>
+      <c r="H12" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>766877</v>
       </c>
@@ -10447,7 +10883,7 @@
         <v>3.0675080000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -10465,9 +10901,9 @@
         <v>262592</v>
       </c>
       <c r="F13" s="7">
-        <v>7701500</v>
-      </c>
-      <c r="H13" s="11">
+        <v>7026600</v>
+      </c>
+      <c r="H13" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>12592</v>
       </c>
@@ -10494,9 +10930,9 @@
         <v>100834480</v>
       </c>
       <c r="F14" s="7">
-        <v>88495300</v>
-      </c>
-      <c r="H14" s="11">
+        <v>92804600</v>
+      </c>
+      <c r="H14" s="12">
         <f>Table1[[#This Row],[Key Comparison]]-Table1[[#This Row],[Edges]]</f>
         <v>75834480</v>
       </c>
@@ -10505,7 +10941,7 @@
         <v>3.0333792000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -10523,7 +10959,7 @@
         <v>25158844</v>
       </c>
       <c r="F15" s="7">
-        <v>404758400</v>
+        <v>506694600</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -10534,19 +10970,19 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="7">
-        <v>198</v>
+        <v>138</v>
       </c>
       <c r="F16" s="7">
-        <v>215400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" hidden="1">
+        <v>206700</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -10554,16 +10990,16 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="7">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="F17" s="7">
-        <v>255400</v>
+        <v>218400</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -10574,19 +11010,19 @@
         <v>100</v>
       </c>
       <c r="C18">
-        <v>4544</v>
+        <v>1966</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="7">
-        <v>35021</v>
+        <v>29361</v>
       </c>
       <c r="F18" s="7">
-        <v>485200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1">
+        <v>410000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -10594,16 +11030,16 @@
         <v>100</v>
       </c>
       <c r="C19">
-        <v>4544</v>
+        <v>1966</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
       </c>
       <c r="E19" s="7">
-        <v>6893</v>
+        <v>4291</v>
       </c>
       <c r="F19" s="7">
-        <v>772300</v>
+        <v>557200</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -10614,19 +11050,19 @@
         <v>1000</v>
       </c>
       <c r="C20">
-        <v>450194</v>
+        <v>199700</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
       </c>
       <c r="E20" s="7">
-        <v>4190113</v>
+        <v>3850228</v>
       </c>
       <c r="F20" s="7">
-        <v>6194100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" hidden="1">
+        <v>4938400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -10634,16 +11070,16 @@
         <v>1000</v>
       </c>
       <c r="C21">
-        <v>450194</v>
+        <v>199700</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
       </c>
       <c r="E21" s="7">
-        <v>485108</v>
+        <v>228345</v>
       </c>
       <c r="F21" s="7">
-        <v>13952300</v>
+        <v>9966300</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -10654,19 +11090,19 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>194</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
       </c>
       <c r="E22" s="7">
-        <v>965</v>
+        <v>739</v>
       </c>
       <c r="F22" s="7">
-        <v>129900</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" hidden="1">
+        <v>167000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -10674,16 +11110,16 @@
         <v>20</v>
       </c>
       <c r="C23">
-        <v>194</v>
+        <v>76</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="7">
-        <v>491</v>
+        <v>295</v>
       </c>
       <c r="F23" s="7">
-        <v>214900</v>
+        <v>174900</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -10694,19 +11130,19 @@
         <v>40</v>
       </c>
       <c r="C24">
-        <v>717</v>
+        <v>356</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="7">
-        <v>4540</v>
+        <v>3776</v>
       </c>
       <c r="F24" s="7">
-        <v>169200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" hidden="1">
+        <v>225300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -10714,16 +11150,16 @@
         <v>40</v>
       </c>
       <c r="C25">
-        <v>717</v>
+        <v>356</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="7">
-        <v>1439</v>
+        <v>1106</v>
       </c>
       <c r="F25" s="7">
-        <v>177900</v>
+        <v>177400</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -10734,19 +11170,19 @@
         <v>500</v>
       </c>
       <c r="C26">
-        <v>112486</v>
+        <v>49787</v>
       </c>
       <c r="D26" t="s">
         <v>0</v>
       </c>
       <c r="E26" s="7">
-        <v>982006</v>
+        <v>953380</v>
       </c>
       <c r="F26" s="7">
-        <v>1720200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" hidden="1">
+        <v>1423600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -10754,16 +11190,16 @@
         <v>500</v>
       </c>
       <c r="C27">
-        <v>112486</v>
+        <v>49787</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
       </c>
       <c r="E27" s="7">
-        <v>126910</v>
+        <v>64486</v>
       </c>
       <c r="F27" s="7">
-        <v>2184900</v>
+        <v>1571200</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -10774,19 +11210,19 @@
         <v>5000</v>
       </c>
       <c r="C28">
-        <v>11244751</v>
+        <v>4999902</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
       </c>
       <c r="E28" s="7">
-        <v>110211671</v>
+        <v>107385202</v>
       </c>
       <c r="F28" s="7">
-        <v>152229900</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" hidden="1">
+        <v>124015400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -10794,16 +11230,16 @@
         <v>5000</v>
       </c>
       <c r="C29">
-        <v>11244751</v>
+        <v>4999902</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
       <c r="E29" s="7">
-        <v>11407621</v>
+        <v>5213390</v>
       </c>
       <c r="F29" s="7">
-        <v>199905000</v>
+        <v>97872700</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -10820,7 +11256,7 @@
         <v>20</v>
       </c>
       <c r="E30">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>400</v>
       </c>
       <c r="H30">
@@ -10842,7 +11278,7 @@
         <v>20</v>
       </c>
       <c r="E31">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>1600</v>
       </c>
     </row>
@@ -10860,7 +11296,7 @@
         <v>20</v>
       </c>
       <c r="E32">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>6400</v>
       </c>
     </row>
@@ -10878,7 +11314,7 @@
         <v>20</v>
       </c>
       <c r="E33">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>40000</v>
       </c>
     </row>
@@ -10896,7 +11332,7 @@
         <v>20</v>
       </c>
       <c r="E34">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>1000000</v>
       </c>
     </row>
@@ -10914,7 +11350,7 @@
         <v>20</v>
       </c>
       <c r="E35">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>4000000</v>
       </c>
     </row>
@@ -10932,7 +11368,7 @@
         <v>20</v>
       </c>
       <c r="E36">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>100000000</v>
       </c>
     </row>
@@ -10944,14 +11380,17 @@
         <v>10</v>
       </c>
       <c r="C37">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="D37" t="s">
         <v>20</v>
       </c>
       <c r="E37">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>400</v>
+      </c>
+      <c r="H37" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -10962,13 +11401,13 @@
         <v>20</v>
       </c>
       <c r="C38">
-        <v>194</v>
+        <v>400</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
       </c>
       <c r="E38">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>1600</v>
       </c>
     </row>
@@ -10980,13 +11419,13 @@
         <v>40</v>
       </c>
       <c r="C39">
-        <v>717</v>
+        <v>1600</v>
       </c>
       <c r="D39" t="s">
         <v>20</v>
       </c>
       <c r="E39">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>6400</v>
       </c>
     </row>
@@ -10998,13 +11437,13 @@
         <v>100</v>
       </c>
       <c r="C40">
-        <v>4544</v>
+        <v>10000</v>
       </c>
       <c r="D40" t="s">
         <v>20</v>
       </c>
       <c r="E40">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>40000</v>
       </c>
     </row>
@@ -11016,13 +11455,13 @@
         <v>500</v>
       </c>
       <c r="C41">
-        <v>112486</v>
+        <v>250000</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
       </c>
       <c r="E41">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>1000000</v>
       </c>
     </row>
@@ -11034,13 +11473,13 @@
         <v>1000</v>
       </c>
       <c r="C42">
-        <v>450194</v>
+        <v>1000000</v>
       </c>
       <c r="D42" t="s">
         <v>20</v>
       </c>
       <c r="E42">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>4000000</v>
       </c>
       <c r="J42" t="s">
@@ -11055,13 +11494,13 @@
         <v>5000</v>
       </c>
       <c r="C43">
-        <v>11244751</v>
+        <v>25000000</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
       </c>
       <c r="E43">
-        <f>2*Table1[[#This Row],[Nvertices]]*(2*Table1[[#This Row],[Nvertices]])</f>
+        <f>4*Table1[[#This Row],[Edges]]</f>
         <v>100000000</v>
       </c>
       <c r="J43" t="s">
@@ -11084,7 +11523,7 @@
         <v>222</v>
       </c>
       <c r="U43" t="str">
-        <v>12311800</v>
+        <v>1584300</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -11101,8 +11540,8 @@
         <v>21</v>
       </c>
       <c r="E44" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>232.8771237954945</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>233</v>
       </c>
       <c r="F44" s="5"/>
       <c r="I44" t="s">
@@ -11128,7 +11567,7 @@
         <v>213</v>
       </c>
       <c r="U44" t="str">
-        <v>1774100</v>
+        <v>1422200</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -11145,8 +11584,8 @@
         <v>21</v>
       </c>
       <c r="E45" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>745.75424759098905</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>746</v>
       </c>
       <c r="F45" s="5"/>
       <c r="P45" s="1" t="s">
@@ -11166,7 +11605,7 @@
         <v>35277</v>
       </c>
       <c r="U45" t="str">
-        <v>2886900</v>
+        <v>3336700</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -11183,8 +11622,8 @@
         <v>21</v>
       </c>
       <c r="E46" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>2451.5084951819781</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>2452</v>
       </c>
       <c r="F46" s="5"/>
       <c r="P46" s="1" t="s">
@@ -11204,7 +11643,7 @@
         <v>12143</v>
       </c>
       <c r="U46" t="str">
-        <v>2933400</v>
+        <v>2892700</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -11221,8 +11660,8 @@
         <v>21</v>
       </c>
       <c r="E47" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>12657.54247590989</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>12658</v>
       </c>
       <c r="F47" s="5"/>
       <c r="P47" s="1" t="s">
@@ -11242,7 +11681,7 @@
         <v>4029793</v>
       </c>
       <c r="U47" t="str">
-        <v>32070100</v>
+        <v>42019700</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -11259,8 +11698,8 @@
         <v>21</v>
       </c>
       <c r="E48" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>267931.56856932415</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>267932</v>
       </c>
       <c r="F48" s="5"/>
       <c r="I48" s="4" t="s">
@@ -11283,7 +11722,7 @@
         <v>1027040</v>
       </c>
       <c r="U48" t="str">
-        <v>64510700</v>
+        <v>59701400</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -11300,8 +11739,8 @@
         <v>21</v>
       </c>
       <c r="E49" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>1039863.1371386483</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>1039864</v>
       </c>
       <c r="F49" s="5"/>
       <c r="P49" s="1" t="s">
@@ -11321,7 +11760,7 @@
         <v>1253</v>
       </c>
       <c r="U49" t="str">
-        <v>257200</v>
+        <v>430100</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -11338,8 +11777,8 @@
         <v>21</v>
       </c>
       <c r="E50" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>25245754.247590989</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>25245755</v>
       </c>
       <c r="F50" s="5"/>
       <c r="P50" s="1" t="s">
@@ -11359,7 +11798,7 @@
         <v>740</v>
       </c>
       <c r="U50" t="str">
-        <v>333200</v>
+        <v>378600</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -11370,14 +11809,14 @@
         <v>10</v>
       </c>
       <c r="C51">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="D51" t="s">
         <v>21</v>
       </c>
       <c r="E51" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>164.44850683942991</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>94</v>
       </c>
       <c r="F51" s="5"/>
       <c r="H51" s="6"/>
@@ -11398,7 +11837,7 @@
         <v>5352</v>
       </c>
       <c r="U51" t="str">
-        <v>257800</v>
+        <v>246900</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -11409,14 +11848,14 @@
         <v>20</v>
       </c>
       <c r="C52">
-        <v>194</v>
+        <v>76</v>
       </c>
       <c r="D52" t="s">
         <v>21</v>
       </c>
       <c r="E52" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>497.99651368748511</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>326</v>
       </c>
       <c r="F52" s="5"/>
       <c r="P52" s="1" t="s">
@@ -11436,7 +11875,7 @@
         <v>2266</v>
       </c>
       <c r="U52" t="str">
-        <v>532000</v>
+        <v>339300</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -11447,14 +11886,14 @@
         <v>40</v>
       </c>
       <c r="C53">
-        <v>717</v>
+        <v>356</v>
       </c>
       <c r="D53" t="s">
         <v>21</v>
       </c>
       <c r="E53" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>1475.8663446961523</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>1035</v>
       </c>
       <c r="F53" s="5"/>
       <c r="P53" s="1" t="s">
@@ -11474,7 +11913,7 @@
         <v>1016877</v>
       </c>
       <c r="U53" t="str">
-        <v>3049200</v>
+        <v>4079000</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -11485,14 +11924,14 @@
         <v>100</v>
       </c>
       <c r="C54">
-        <v>4544</v>
+        <v>1966</v>
       </c>
       <c r="D54" t="s">
         <v>21</v>
       </c>
       <c r="E54" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>6973.9494239009364</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>4155</v>
       </c>
       <c r="F54" s="5"/>
       <c r="P54" s="1" t="s">
@@ -11512,7 +11951,7 @@
         <v>262592</v>
       </c>
       <c r="U54" t="str">
-        <v>7701500</v>
+        <v>7026600</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -11523,14 +11962,14 @@
         <v>500</v>
       </c>
       <c r="C55">
-        <v>112486</v>
+        <v>49787</v>
       </c>
       <c r="D55" t="s">
         <v>21</v>
       </c>
       <c r="E55" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>129265.38592932424</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>65391</v>
       </c>
       <c r="F55" s="5"/>
       <c r="P55" s="1" t="s">
@@ -11550,7 +11989,7 @@
         <v>100834480</v>
       </c>
       <c r="U55" t="str">
-        <v>88495300</v>
+        <v>92804600</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -11561,14 +12000,14 @@
         <v>1000</v>
       </c>
       <c r="C56">
-        <v>450194</v>
+        <v>199700</v>
       </c>
       <c r="D56" t="s">
         <v>21</v>
       </c>
       <c r="E56" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>487754.37460742478</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>234915</v>
       </c>
       <c r="F56" s="5"/>
       <c r="P56" s="1" t="s">
@@ -11588,7 +12027,7 @@
         <v>25158844</v>
       </c>
       <c r="U56" t="str">
-        <v>404758400</v>
+        <v>506694600</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -11599,14 +12038,14 @@
         <v>5000</v>
       </c>
       <c r="C57">
-        <v>11244751</v>
+        <v>4999902</v>
       </c>
       <c r="D57" t="s">
         <v>21</v>
       </c>
       <c r="E57" s="5">
-        <f>(Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2)</f>
-        <v>11478978.483791253</v>
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Edges]])+2*(Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Edges]],2))</f>
+        <v>5222437</v>
       </c>
       <c r="F57" s="5"/>
       <c r="P57" s="1" t="s">
@@ -11623,13 +12062,29 @@
         <v>Array</v>
       </c>
       <c r="T57" t="str">
-        <v>198</v>
+        <v>138</v>
       </c>
       <c r="U57" t="str">
-        <v>215400</v>
+        <v>206700</v>
       </c>
     </row>
     <row r="58" spans="1:21">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>100</v>
+      </c>
+      <c r="D58" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>100</v>
+      </c>
       <c r="P58" s="1" t="s">
         <v>38</v>
       </c>
@@ -11644,13 +12099,29 @@
         <v>Heap</v>
       </c>
       <c r="T58" t="str">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="U58" t="str">
-        <v>255400</v>
+        <v>218400</v>
       </c>
     </row>
     <row r="59" spans="1:21">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59">
+        <v>20</v>
+      </c>
+      <c r="C59">
+        <v>400</v>
+      </c>
+      <c r="D59" t="s">
+        <v>52</v>
+      </c>
+      <c r="E59" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>400</v>
+      </c>
       <c r="P59" s="1" t="s">
         <v>39</v>
       </c>
@@ -11665,13 +12136,29 @@
         <v>Array</v>
       </c>
       <c r="T59" t="str">
-        <v>35021</v>
+        <v>29361</v>
       </c>
       <c r="U59" t="str">
-        <v>485200</v>
+        <v>410000</v>
       </c>
     </row>
     <row r="60" spans="1:21">
+      <c r="A60" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60">
+        <v>40</v>
+      </c>
+      <c r="C60">
+        <v>1600</v>
+      </c>
+      <c r="D60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>1600</v>
+      </c>
       <c r="P60" s="1" t="s">
         <v>40</v>
       </c>
@@ -11686,13 +12173,29 @@
         <v>Heap</v>
       </c>
       <c r="T60" t="str">
-        <v>6893</v>
+        <v>4291</v>
       </c>
       <c r="U60" t="str">
-        <v>772300</v>
+        <v>557200</v>
       </c>
     </row>
     <row r="61" spans="1:21">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61">
+        <v>100</v>
+      </c>
+      <c r="C61">
+        <v>10000</v>
+      </c>
+      <c r="D61" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>10000</v>
+      </c>
       <c r="P61" s="1" t="s">
         <v>41</v>
       </c>
@@ -11707,13 +12210,29 @@
         <v>Array</v>
       </c>
       <c r="T61" t="str">
-        <v>4190113</v>
+        <v>3850228</v>
       </c>
       <c r="U61" t="str">
-        <v>6194100</v>
+        <v>4938400</v>
       </c>
     </row>
     <row r="62" spans="1:21">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <v>500</v>
+      </c>
+      <c r="C62">
+        <v>250000</v>
+      </c>
+      <c r="D62" t="s">
+        <v>52</v>
+      </c>
+      <c r="E62" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>250000</v>
+      </c>
       <c r="P62" s="1" t="s">
         <v>42</v>
       </c>
@@ -11728,13 +12247,29 @@
         <v>Heap</v>
       </c>
       <c r="T62" t="str">
-        <v>485108</v>
+        <v>228345</v>
       </c>
       <c r="U62" t="str">
-        <v>13952300</v>
+        <v>9966300</v>
       </c>
     </row>
     <row r="63" spans="1:21">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63">
+        <v>1000</v>
+      </c>
+      <c r="C63">
+        <v>1000000</v>
+      </c>
+      <c r="D63" t="s">
+        <v>52</v>
+      </c>
+      <c r="E63" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>1000000</v>
+      </c>
       <c r="P63" s="1" t="s">
         <v>43</v>
       </c>
@@ -11749,13 +12284,29 @@
         <v>Array</v>
       </c>
       <c r="T63" t="str">
-        <v>965</v>
+        <v>739</v>
       </c>
       <c r="U63" t="str">
-        <v>129900</v>
+        <v>167000</v>
       </c>
     </row>
     <row r="64" spans="1:21">
+      <c r="A64" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64">
+        <v>5000</v>
+      </c>
+      <c r="C64">
+        <v>25000000</v>
+      </c>
+      <c r="D64" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>25000000</v>
+      </c>
       <c r="P64" s="1" t="s">
         <v>44</v>
       </c>
@@ -11770,13 +12321,29 @@
         <v>Heap</v>
       </c>
       <c r="T64" t="str">
-        <v>491</v>
+        <v>295</v>
       </c>
       <c r="U64" t="str">
-        <v>214900</v>
-      </c>
-    </row>
-    <row r="65" spans="16:21">
+        <v>174900</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>10</v>
+      </c>
+      <c r="C65">
+        <v>100</v>
+      </c>
+      <c r="D65" t="s">
+        <v>52</v>
+      </c>
+      <c r="E65" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>100</v>
+      </c>
       <c r="P65" s="1" t="s">
         <v>45</v>
       </c>
@@ -11791,13 +12358,29 @@
         <v>Array</v>
       </c>
       <c r="T65" t="str">
-        <v>4540</v>
+        <v>3776</v>
       </c>
       <c r="U65" t="str">
-        <v>169200</v>
-      </c>
-    </row>
-    <row r="66" spans="16:21">
+        <v>225300</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>20</v>
+      </c>
+      <c r="C66">
+        <v>400</v>
+      </c>
+      <c r="D66" t="s">
+        <v>52</v>
+      </c>
+      <c r="E66" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>400</v>
+      </c>
       <c r="P66" s="1" t="s">
         <v>46</v>
       </c>
@@ -11812,13 +12395,29 @@
         <v>Heap</v>
       </c>
       <c r="T66" t="str">
-        <v>1439</v>
+        <v>1106</v>
       </c>
       <c r="U66" t="str">
-        <v>177900</v>
-      </c>
-    </row>
-    <row r="67" spans="16:21">
+        <v>177400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>40</v>
+      </c>
+      <c r="C67">
+        <v>1600</v>
+      </c>
+      <c r="D67" t="s">
+        <v>52</v>
+      </c>
+      <c r="E67" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>1600</v>
+      </c>
       <c r="P67" s="1" t="s">
         <v>47</v>
       </c>
@@ -11833,13 +12432,29 @@
         <v>Array</v>
       </c>
       <c r="T67" t="str">
-        <v>982006</v>
+        <v>953380</v>
       </c>
       <c r="U67" t="str">
-        <v>1720200</v>
-      </c>
-    </row>
-    <row r="68" spans="16:21">
+        <v>1423600</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>100</v>
+      </c>
+      <c r="C68">
+        <v>10000</v>
+      </c>
+      <c r="D68" t="s">
+        <v>52</v>
+      </c>
+      <c r="E68" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>10000</v>
+      </c>
       <c r="P68" s="1" t="s">
         <v>48</v>
       </c>
@@ -11854,13 +12469,29 @@
         <v>Heap</v>
       </c>
       <c r="T68" t="str">
-        <v>126910</v>
+        <v>64486</v>
       </c>
       <c r="U68" t="str">
-        <v>2184900</v>
-      </c>
-    </row>
-    <row r="69" spans="16:21">
+        <v>1571200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>500</v>
+      </c>
+      <c r="C69">
+        <v>250000</v>
+      </c>
+      <c r="D69" t="s">
+        <v>52</v>
+      </c>
+      <c r="E69" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>250000</v>
+      </c>
       <c r="P69" s="1" t="s">
         <v>49</v>
       </c>
@@ -11875,13 +12506,29 @@
         <v>Array</v>
       </c>
       <c r="T69" t="str">
-        <v>110211671</v>
+        <v>107385202</v>
       </c>
       <c r="U69" t="str">
-        <v>152229900</v>
-      </c>
-    </row>
-    <row r="70" spans="16:21">
+        <v>124015400</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>1000</v>
+      </c>
+      <c r="C70">
+        <v>1000000</v>
+      </c>
+      <c r="D70" t="s">
+        <v>52</v>
+      </c>
+      <c r="E70" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>1000000</v>
+      </c>
       <c r="P70" s="1" t="s">
         <v>50</v>
       </c>
@@ -11896,10 +12543,280 @@
         <v>Heap</v>
       </c>
       <c r="T70" t="str">
-        <v>11407621</v>
+        <v>5213390</v>
       </c>
       <c r="U70" t="str">
-        <v>199905000</v>
+        <v>97872700</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>5000</v>
+      </c>
+      <c r="C71">
+        <v>25000000</v>
+      </c>
+      <c r="D71" t="s">
+        <v>52</v>
+      </c>
+      <c r="E71" s="5">
+        <f>Table1[[#This Row],[Edges]]</f>
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21">
+      <c r="A72" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>100</v>
+      </c>
+      <c r="D72" t="s">
+        <v>53</v>
+      </c>
+      <c r="E72" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21">
+      <c r="A73" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73">
+        <v>20</v>
+      </c>
+      <c r="C73">
+        <v>400</v>
+      </c>
+      <c r="D73" t="s">
+        <v>53</v>
+      </c>
+      <c r="E73" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74">
+        <v>40</v>
+      </c>
+      <c r="C74">
+        <v>1600</v>
+      </c>
+      <c r="D74" t="s">
+        <v>53</v>
+      </c>
+      <c r="E74" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21">
+      <c r="A75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75">
+        <v>100</v>
+      </c>
+      <c r="C75">
+        <v>10000</v>
+      </c>
+      <c r="D75" t="s">
+        <v>53</v>
+      </c>
+      <c r="E75" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>665</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21">
+      <c r="A76" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76">
+        <v>500</v>
+      </c>
+      <c r="C76">
+        <v>250000</v>
+      </c>
+      <c r="D76" t="s">
+        <v>53</v>
+      </c>
+      <c r="E76" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>4483</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21">
+      <c r="A77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77">
+        <v>1000</v>
+      </c>
+      <c r="C77">
+        <v>1000000</v>
+      </c>
+      <c r="D77" t="s">
+        <v>53</v>
+      </c>
+      <c r="E77" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>9966</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21">
+      <c r="A78" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78">
+        <v>5000</v>
+      </c>
+      <c r="C78">
+        <v>25000000</v>
+      </c>
+      <c r="D78" t="s">
+        <v>53</v>
+      </c>
+      <c r="E78" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>61439</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <v>15</v>
+      </c>
+      <c r="D79" t="s">
+        <v>53</v>
+      </c>
+      <c r="E79" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80">
+        <v>20</v>
+      </c>
+      <c r="C80">
+        <v>76</v>
+      </c>
+      <c r="D80" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>40</v>
+      </c>
+      <c r="C81">
+        <v>356</v>
+      </c>
+      <c r="D81" t="s">
+        <v>53</v>
+      </c>
+      <c r="E81" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82">
+        <v>100</v>
+      </c>
+      <c r="C82">
+        <v>1966</v>
+      </c>
+      <c r="D82" t="s">
+        <v>53</v>
+      </c>
+      <c r="E82" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>665</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>500</v>
+      </c>
+      <c r="C83">
+        <v>49787</v>
+      </c>
+      <c r="D83" t="s">
+        <v>53</v>
+      </c>
+      <c r="E83" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>4483</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84">
+        <v>1000</v>
+      </c>
+      <c r="C84">
+        <v>199700</v>
+      </c>
+      <c r="D84" t="s">
+        <v>53</v>
+      </c>
+      <c r="E84" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>9966</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>5000</v>
+      </c>
+      <c r="C85">
+        <v>4999902</v>
+      </c>
+      <c r="D85" t="s">
+        <v>53</v>
+      </c>
+      <c r="E85" s="5">
+        <f>_xlfn.CEILING.MATH((Table1[[#This Row],[Nvertices]])*LOG(Table1[[#This Row],[Nvertices]],2))</f>
+        <v>61439</v>
       </c>
     </row>
   </sheetData>
@@ -11918,256 +12835,524 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47ACD059-68C1-48DD-91E4-F967774AC188}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="F46" sqref="F46:H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A2" s="8">
-        <v>213</v>
-      </c>
-      <c r="B2" s="9">
-        <v>233</v>
-      </c>
-      <c r="C2">
-        <f>100-(A2/B2)*100</f>
-        <v>8.5836909871244558</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A3" s="8">
-        <v>740</v>
-      </c>
-      <c r="B3" s="9">
-        <v>746</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C33" si="0">100-(A3/B3)*100</f>
-        <v>0.80428954423592813</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A4" s="8">
-        <v>2266</v>
-      </c>
-      <c r="B4" s="9">
-        <v>2452</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>7.5856443719412709</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A5" s="8">
-        <v>12143</v>
-      </c>
-      <c r="B5" s="9">
-        <v>12658</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>4.0685732343182224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A6" s="8">
-        <v>262592</v>
-      </c>
-      <c r="B6" s="9">
-        <v>267932</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>1.993043010913226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A7" s="8">
-        <v>1027040</v>
-      </c>
-      <c r="B7" s="9">
-        <v>1039863</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>1.2331432121346779</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A8" s="8">
-        <v>25158844</v>
-      </c>
-      <c r="B8" s="9">
-        <v>25245754</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0.344255909330343</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="C9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" t="e">
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="12"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="13"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="12"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="13"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="12"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="13"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="12"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="13"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="12"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="13"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="12"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="13"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="12"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="13"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="E36" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="14"/>
+      <c r="I36" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="E37" s="3">
+        <v>10</v>
+      </c>
+      <c r="F37" s="7">
+        <v>222</v>
+      </c>
+      <c r="G37" s="7">
+        <v>400</v>
+      </c>
+      <c r="H37" s="15">
+        <f>100-(F37/G37)*100</f>
+        <v>44.499999999999993</v>
+      </c>
+      <c r="I37" s="7">
+        <v>213</v>
+      </c>
+      <c r="J37" s="7">
+        <v>233</v>
+      </c>
+      <c r="K37" s="15">
+        <f>100-(I37/J37)*100</f>
+        <v>8.5836909871244558</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="E38" s="3">
+        <v>20</v>
+      </c>
+      <c r="F38" s="7">
+        <v>1253</v>
+      </c>
+      <c r="G38" s="7">
+        <v>1600</v>
+      </c>
+      <c r="H38" s="15">
+        <f t="shared" ref="H38:H43" si="0">100-(F38/G38)*100</f>
+        <v>21.6875</v>
+      </c>
+      <c r="I38" s="7">
+        <v>740</v>
+      </c>
+      <c r="J38" s="7">
+        <v>746</v>
+      </c>
+      <c r="K38" s="15">
+        <f t="shared" ref="K38:K43" si="1">100-(I38/J38)*100</f>
+        <v>0.80428954423592813</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="E39" s="3">
+        <v>40</v>
+      </c>
+      <c r="F39" s="7">
+        <v>5352</v>
+      </c>
+      <c r="G39" s="7">
+        <v>6400</v>
+      </c>
+      <c r="H39" s="15">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A11" s="8">
-        <v>132</v>
-      </c>
-      <c r="B11" s="9">
-        <v>164</v>
-      </c>
-      <c r="C11">
+        <v>16.375</v>
+      </c>
+      <c r="I39" s="7">
+        <v>2266</v>
+      </c>
+      <c r="J39" s="7">
+        <v>2452</v>
+      </c>
+      <c r="K39" s="15">
+        <f t="shared" si="1"/>
+        <v>7.5856443719412709</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="E40" s="3">
+        <v>100</v>
+      </c>
+      <c r="F40" s="7">
+        <v>35277</v>
+      </c>
+      <c r="G40" s="7">
+        <v>40000</v>
+      </c>
+      <c r="H40" s="15">
         <f t="shared" si="0"/>
-        <v>19.512195121951208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A12" s="8">
-        <v>491</v>
-      </c>
-      <c r="B12" s="9">
-        <v>498</v>
-      </c>
-      <c r="C12">
+        <v>11.807500000000005</v>
+      </c>
+      <c r="I40" s="7">
+        <v>12143</v>
+      </c>
+      <c r="J40" s="7">
+        <v>12658</v>
+      </c>
+      <c r="K40" s="15">
+        <f t="shared" si="1"/>
+        <v>4.0685732343182224</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="E41" s="3">
+        <v>500</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1016877</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="H41" s="15">
         <f t="shared" si="0"/>
-        <v>1.4056224899598391</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A13" s="8">
-        <v>1439</v>
-      </c>
-      <c r="B13" s="9">
-        <v>1476</v>
-      </c>
-      <c r="C13">
+        <v>-1.6877000000000066</v>
+      </c>
+      <c r="I41" s="7">
+        <v>262592</v>
+      </c>
+      <c r="J41" s="7">
+        <v>267932</v>
+      </c>
+      <c r="K41" s="15">
+        <f t="shared" si="1"/>
+        <v>1.993043010913226</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="E42" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F42" s="7">
+        <v>4029793</v>
+      </c>
+      <c r="G42" s="7">
+        <v>4000000</v>
+      </c>
+      <c r="H42" s="15">
         <f t="shared" si="0"/>
-        <v>2.5067750677506808</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A14" s="8">
-        <v>6893</v>
-      </c>
-      <c r="B14" s="9">
-        <v>6974</v>
-      </c>
-      <c r="C14">
+        <v>-0.74482499999999163</v>
+      </c>
+      <c r="I42" s="7">
+        <v>1027040</v>
+      </c>
+      <c r="J42" s="7">
+        <v>1039864</v>
+      </c>
+      <c r="K42" s="15">
+        <f t="shared" si="1"/>
+        <v>1.2332381926867413</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="E43" s="3">
+        <v>5000</v>
+      </c>
+      <c r="F43" s="7">
+        <v>100834480</v>
+      </c>
+      <c r="G43" s="7">
+        <v>100000000</v>
+      </c>
+      <c r="H43" s="15">
         <f t="shared" si="0"/>
-        <v>1.161456839690274</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A15" s="8">
-        <v>126910</v>
-      </c>
-      <c r="B15" s="9">
-        <v>129265</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>1.8218388581595946</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A16" s="8">
-        <v>485108</v>
-      </c>
-      <c r="B16" s="9">
-        <v>487754</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>0.54248658135043115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A17" s="8">
-        <v>11407621</v>
-      </c>
-      <c r="B17" s="9">
-        <v>11478978</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>0.62163199546161252</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="C18" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="C19" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="11"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="12"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="12"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="11"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="12"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="11"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="12"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="11"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="12"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="11"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="12"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="11"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="12"/>
+        <v>-0.83447999999999922</v>
+      </c>
+      <c r="I43" s="7">
+        <v>25158844</v>
+      </c>
+      <c r="J43" s="7">
+        <v>25245755</v>
+      </c>
+      <c r="K43" s="15">
+        <f t="shared" si="1"/>
+        <v>0.34425985675611059</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="E44" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="15"/>
+      <c r="K44" s="15"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="E45" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" s="14"/>
+      <c r="I45" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="15"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="E46" s="3">
+        <v>10</v>
+      </c>
+      <c r="F46" s="7">
+        <v>138</v>
+      </c>
+      <c r="G46" s="7">
+        <v>400</v>
+      </c>
+      <c r="H46" s="15">
+        <f t="shared" ref="H46:H52" si="2">100-(F46/G46)*100</f>
+        <v>65.5</v>
+      </c>
+      <c r="I46" s="7">
+        <v>66</v>
+      </c>
+      <c r="J46" s="7">
+        <v>94</v>
+      </c>
+      <c r="K46" s="15">
+        <f t="shared" ref="K46:K52" si="3">100-(I46/J46)*100</f>
+        <v>29.787234042553195</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="E47" s="3">
+        <v>20</v>
+      </c>
+      <c r="F47" s="7">
+        <v>739</v>
+      </c>
+      <c r="G47" s="7">
+        <v>1600</v>
+      </c>
+      <c r="H47" s="15">
+        <f t="shared" si="2"/>
+        <v>53.8125</v>
+      </c>
+      <c r="I47" s="7">
+        <v>295</v>
+      </c>
+      <c r="J47" s="7">
+        <v>326</v>
+      </c>
+      <c r="K47" s="15">
+        <f t="shared" si="3"/>
+        <v>9.5092024539877258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="E48" s="3">
+        <v>40</v>
+      </c>
+      <c r="F48" s="7">
+        <v>3776</v>
+      </c>
+      <c r="G48" s="7">
+        <v>6400</v>
+      </c>
+      <c r="H48" s="15">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="I48" s="7">
+        <v>1106</v>
+      </c>
+      <c r="J48" s="7">
+        <v>1035</v>
+      </c>
+      <c r="K48" s="15">
+        <f t="shared" si="3"/>
+        <v>-6.8599033816425106</v>
+      </c>
+    </row>
+    <row r="49" spans="5:11">
+      <c r="E49" s="3">
+        <v>100</v>
+      </c>
+      <c r="F49" s="7">
+        <v>29361</v>
+      </c>
+      <c r="G49" s="7">
+        <v>40000</v>
+      </c>
+      <c r="H49" s="15">
+        <f t="shared" si="2"/>
+        <v>26.597499999999997</v>
+      </c>
+      <c r="I49" s="7">
+        <v>4291</v>
+      </c>
+      <c r="J49" s="7">
+        <v>4155</v>
+      </c>
+      <c r="K49" s="15">
+        <f t="shared" si="3"/>
+        <v>-3.2731648616125142</v>
+      </c>
+    </row>
+    <row r="50" spans="5:11">
+      <c r="E50" s="3">
+        <v>500</v>
+      </c>
+      <c r="F50" s="7">
+        <v>953380</v>
+      </c>
+      <c r="G50" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="H50" s="15">
+        <f t="shared" si="2"/>
+        <v>4.6620000000000061</v>
+      </c>
+      <c r="I50" s="7">
+        <v>64486</v>
+      </c>
+      <c r="J50" s="7">
+        <v>65391</v>
+      </c>
+      <c r="K50" s="15">
+        <f t="shared" si="3"/>
+        <v>1.383982505237725</v>
+      </c>
+    </row>
+    <row r="51" spans="5:11">
+      <c r="E51" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F51" s="7">
+        <v>3850228</v>
+      </c>
+      <c r="G51" s="7">
+        <v>4000000</v>
+      </c>
+      <c r="H51" s="15">
+        <f t="shared" si="2"/>
+        <v>3.7442999999999955</v>
+      </c>
+      <c r="I51" s="7">
+        <v>228345</v>
+      </c>
+      <c r="J51" s="7">
+        <v>234915</v>
+      </c>
+      <c r="K51" s="15">
+        <f t="shared" si="3"/>
+        <v>2.7967562735457534</v>
+      </c>
+    </row>
+    <row r="52" spans="5:11">
+      <c r="E52" s="3">
+        <v>5000</v>
+      </c>
+      <c r="F52" s="7">
+        <v>107385202</v>
+      </c>
+      <c r="G52" s="7">
+        <v>100000000</v>
+      </c>
+      <c r="H52" s="15">
+        <f t="shared" si="2"/>
+        <v>-7.3852019999999925</v>
+      </c>
+      <c r="I52" s="7">
+        <v>5213390</v>
+      </c>
+      <c r="J52" s="7">
+        <v>5222437</v>
+      </c>
+      <c r="K52" s="15">
+        <f t="shared" si="3"/>
+        <v>0.17323330085169175</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>